<commit_message>
added updated NOGAM biomass version
</commit_message>
<xml_diff>
--- a/build_model/input/BIOMASS_RBA.xlsx
+++ b/build_model/input/BIOMASS_RBA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejm6426/Documents/scRBA/build_model/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B7D051-4975-4E40-9649-B494CB6E1062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BB9D30-9609-6349-8ADB-3156CD617DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2680" yWindow="1920" windowWidth="30240" windowHeight="17240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RBABioRxns" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
     <definedName name="TextSplitArray_DIY" comment="Like TEXTSPLIT but for an array; input cells and then a string to split them by. If the input array is a row, it's split vertically; otherwise, it's split horizontally." localSheetId="1">_xlfn.LAMBDA(_xlpm.cells,_xlop.delimiter,_xlfn.LET(_xlpm.str,'batch-Rabinowitz'!IfBlank_DIY(_xlpm.delimiter," "),_xlpm.n,MAX((LEN(_xlpm.cells)-LEN(SUBSTITUTE(_xlpm.cells,_xlpm.str,""))+1)/LEN(_xlpm.str)),_xlfn.TEXTBEFORE(IFERROR(_xlfn.TEXTAFTER(_xlpm.cells,_xlpm.str,IF(COLUMNS(_xlpm.cells)&gt;1,_xlfn.SEQUENCE(_xlpm.n,1,0),_xlfn.SEQUENCE(1,_xlpm.n,0)),,,""),_xlpm.cells),_xlpm.str,,,1,"")))</definedName>
     <definedName name="TextSplitArray_DIY" comment="Like TEXTSPLIT but for an array; input cells and then a string to split them by. If the input array is a row, it's split vertically; otherwise, it's split horizontally.">_xlfn.LAMBDA(_xlpm.cells,_xlop.delimiter,_xlfn.LET(_xlpm.str,IfBlank_DIY(_xlpm.delimiter," "),_xlpm.n,MAX((LEN(_xlpm.cells)-LEN(SUBSTITUTE(_xlpm.cells,_xlpm.str,""))+1)/LEN(_xlpm.str)),_xlfn.TEXTBEFORE(IFERROR(_xlfn.TEXTAFTER(_xlpm.cells,_xlpm.str,IF(COLUMNS(_xlpm.cells)&gt;1,_xlfn.SEQUENCE(_xlpm.n,1,0),_xlfn.SEQUENCE(1,_xlpm.n,0)),,,""),_xlpm.cells),_xlpm.str,,,1,"")))</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -5282,10 +5282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5989,6 +5989,15 @@
       </c>
       <c r="B71" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A72" t="str" cm="1">
+        <f t="array" ref="A72:B72">'batch-Rabinowitz'!Y7:Z7</f>
+        <v>BIOSYN-BIODILAERO-NOGAM</v>
+      </c>
+      <c r="B72" t="str">
+        <v xml:space="preserve">0.933442277567423 BIO-varbiom + 0.00491511903026273 BIO-cofactor + 0.00244129187799933 BIO-dna + 0.020050549978631 BIO-lipid + 0.0257857478364828 BIO-metal + 0.010314301982428 BIO-pi + 0.00305071172677345 BIO-so4 --&gt; </v>
       </c>
     </row>
   </sheetData>
@@ -6005,8 +6014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F168A7-6B4E-494D-BA75-6693E50B2433}">
   <dimension ref="A1:AG95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView topLeftCell="O1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="T12" activeCellId="2" sqref="T6 T13 T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14596,7 +14605,7 @@
   <dimension ref="A1:K111"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="J16" sqref="I16:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
fixed rounding on NOGAM variant
</commit_message>
<xml_diff>
--- a/build_model/input/BIOMASS_RBA.xlsx
+++ b/build_model/input/BIOMASS_RBA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejm6426/Documents/scRBA/build_model/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BB9D30-9609-6349-8ADB-3156CD617DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A104147-8E93-E04A-B712-2E0C3337CA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="1920" windowWidth="30240" windowHeight="17240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RBABioRxns" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="487">
   <si>
     <t>rxn_id</t>
   </si>
@@ -4161,6 +4161,12 @@
   </si>
   <si>
     <t>amount from sheet below</t>
+  </si>
+  <si>
+    <t>BIOSYN-BIODILAERO-NOGAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.933442277567423 BIO-varbiom + 0.020050549978631 BIO-lipid + 0.002441292 BIO-dna + 0.025785748 BIO-metal + 0.004915119 BIO-cofactor + 0.003050712 BIO-so4 + 0.010314302 BIO-pi --&gt; </t>
   </si>
 </sst>
 </file>
@@ -5284,8 +5290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5992,12 +5998,11 @@
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A72" t="str" cm="1">
-        <f t="array" ref="A72:B72">'batch-Rabinowitz'!Y7:Z7</f>
-        <v>BIOSYN-BIODILAERO-NOGAM</v>
-      </c>
-      <c r="B72" t="str">
-        <v xml:space="preserve">0.933442277567423 BIO-varbiom + 0.00491511903026273 BIO-cofactor + 0.00244129187799933 BIO-dna + 0.020050549978631 BIO-lipid + 0.0257857478364828 BIO-metal + 0.010314301982428 BIO-pi + 0.00305071172677345 BIO-so4 --&gt; </v>
+      <c r="A72" t="s">
+        <v>485</v>
+      </c>
+      <c r="B72" t="s">
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -6014,7 +6019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F168A7-6B4E-494D-BA75-6693E50B2433}">
   <dimension ref="A1:AG95"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="T12" activeCellId="2" sqref="T6 T13 T12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
glycogen category changed to carb
</commit_message>
<xml_diff>
--- a/build_model/input/BIOMASS_RBA.xlsx
+++ b/build_model/input/BIOMASS_RBA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejm6426/Documents/scRBA/build_model/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E667E14-E7B2-EC4F-BB16-C854DB60B59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9182E1-9930-264B-8122-C90E8ECA0601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19400" yWindow="0" windowWidth="19000" windowHeight="21600" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19400" yWindow="0" windowWidth="19000" windowHeight="21600" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RBABioRxns" sheetId="1" r:id="rId1"/>
@@ -4951,7 +4951,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CA2C806C-897B-5147-A380-91890FB6F1D0}" name="metaboliteInfo" displayName="metaboliteInfo" ref="A2:E118" totalsRowShown="0">
   <autoFilter ref="A2:E118" xr:uid="{EB067577-3D81-D244-B73F-3CC89BC642F7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E118">
-    <sortCondition ref="A2:A118"/>
+    <sortCondition ref="B2:B118"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{03663191-5848-1A4B-801E-1B9D39F1DF45}" name="name w/o location"/>
@@ -6022,7 +6022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F168A7-6B4E-494D-BA75-6693E50B2433}">
   <dimension ref="A1:AG95"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A55" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
@@ -12793,8 +12793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042FF932-C48A-D446-979E-E5F082761A47}">
   <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A71" sqref="A54:D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12858,1313 +12858,1319 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>332</v>
+        <v>238</v>
       </c>
       <c r="B5" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C5">
-        <v>458.44785999999999</v>
+        <v>203.19252</v>
       </c>
       <c r="D5">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>458.44785999999999</v>
+        <v>203.19252</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>235</v>
       </c>
       <c r="C6">
-        <v>424.177302</v>
+        <v>2619.1368040000002</v>
       </c>
       <c r="D6">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>424.177302</v>
+        <v>2619.1368040000002</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>283</v>
+        <v>339</v>
       </c>
       <c r="B7" t="s">
-        <v>284</v>
+        <v>235</v>
       </c>
       <c r="C7">
-        <v>72.085840000000005</v>
+        <v>162.14060000000001</v>
       </c>
       <c r="D7">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>72.085840000000005</v>
+        <v>162.14060000000001</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B8" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C8">
-        <v>399.44531999999998</v>
+        <v>2280.41334042176</v>
       </c>
       <c r="D8">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>399.44531999999998</v>
+        <v>2280.41334042176</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>285</v>
+        <v>342</v>
       </c>
       <c r="B9" t="s">
-        <v>284</v>
+        <v>235</v>
       </c>
       <c r="C9">
-        <v>158.20156</v>
+        <v>162.14060000000001</v>
       </c>
       <c r="D9">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>158.20156</v>
+        <v>162.14060000000001</v>
+      </c>
+      <c r="E9" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>286</v>
+        <v>240</v>
       </c>
       <c r="B10" t="s">
-        <v>284</v>
+        <v>235</v>
       </c>
       <c r="C10">
-        <v>115.11058</v>
+        <v>810.70299999999997</v>
       </c>
       <c r="D10">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>115.11058</v>
+        <v>810.70299999999997</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>287</v>
+        <v>349</v>
       </c>
       <c r="B11" t="s">
-        <v>284</v>
+        <v>235</v>
       </c>
       <c r="C11">
-        <v>115.0874</v>
+        <v>342.29647999999997</v>
       </c>
       <c r="D11">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>115.0874</v>
+        <v>342.29647999999997</v>
+      </c>
+      <c r="E11" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>304</v>
+        <v>332</v>
       </c>
       <c r="B12" t="s">
-        <v>305</v>
+        <v>242</v>
       </c>
       <c r="C12">
-        <v>503.14926300000002</v>
+        <v>458.44785999999999</v>
       </c>
       <c r="D12">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>328.19800099999998</v>
+        <v>458.44785999999999</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B13" t="s">
         <v>242</v>
       </c>
       <c r="C13">
-        <v>243.30269999999999</v>
+        <v>399.44531999999998</v>
       </c>
       <c r="D13">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>243.30269999999999</v>
+        <v>399.44531999999998</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>273</v>
+        <v>243</v>
       </c>
       <c r="B14" t="s">
-        <v>274</v>
+        <v>242</v>
       </c>
       <c r="C14">
-        <v>40.078000000000003</v>
+        <v>243.30269999999999</v>
       </c>
       <c r="D14">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>40.078000000000003</v>
+        <v>243.30269999999999</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>333</v>
+        <v>244</v>
       </c>
       <c r="B15" t="s">
-        <v>334</v>
+        <v>242</v>
       </c>
       <c r="C15">
-        <v>328.19800099999998</v>
+        <v>763.50236299999995</v>
       </c>
       <c r="D15">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>328.19800099999998</v>
+        <v>763.50236299999995</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="B16" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="C16">
-        <v>203.19252</v>
+        <v>782.52592200000004</v>
       </c>
       <c r="D16">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>203.19252</v>
+        <v>782.52592200000004</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>335</v>
+        <v>246</v>
       </c>
       <c r="B17" t="s">
-        <v>334</v>
+        <v>242</v>
       </c>
       <c r="C17">
-        <v>144970.98955999999</v>
+        <v>850.82126000000005</v>
       </c>
       <c r="D17">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>144970.98955999999</v>
+        <v>850.82126000000005</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B18" t="s">
         <v>242</v>
       </c>
       <c r="C18">
-        <v>763.50236299999995</v>
+        <v>662.41716199999996</v>
       </c>
       <c r="D18">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>763.50236299999995</v>
+        <v>662.41716199999996</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>306</v>
+        <v>479</v>
       </c>
       <c r="B19" t="s">
-        <v>305</v>
+        <v>242</v>
       </c>
       <c r="C19">
-        <v>479.12456300000002</v>
+        <v>663.42510200000004</v>
       </c>
       <c r="D19">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>304.17330100000004</v>
+        <v>663.42510200000004</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>275</v>
+        <v>248</v>
       </c>
       <c r="B20" t="s">
-        <v>274</v>
+        <v>242</v>
       </c>
       <c r="C20">
-        <v>63.545999999999999</v>
+        <v>740.38118299999996</v>
       </c>
       <c r="D20">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>63.545999999999999</v>
+        <v>740.38118299999996</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>288</v>
+        <v>478</v>
       </c>
       <c r="B21" t="s">
-        <v>284</v>
-      </c>
-      <c r="C21">
-        <v>104.15084</v>
+        <v>242</v>
+      </c>
+      <c r="C21" s="49">
+        <v>741.38912300000004</v>
       </c>
       <c r="D21">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>104.15084</v>
+        <v>741.38912300000004</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>242</v>
       </c>
       <c r="C22">
-        <v>487.14986299999998</v>
+        <v>245.126</v>
       </c>
       <c r="D22">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>312.19860099999994</v>
+        <v>245.126</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>242</v>
       </c>
       <c r="C23">
-        <v>463.12516299999999</v>
+        <v>375.35595999999998</v>
       </c>
       <c r="D23">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>288.173901</v>
+        <v>375.35595999999998</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>242</v>
       </c>
       <c r="C24">
-        <v>503.14926300000002</v>
+        <v>148.26967999999999</v>
       </c>
       <c r="D24">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>328.19800099999998</v>
+        <v>148.26967999999999</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B25" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="C25">
-        <v>339.57481999999999</v>
+        <v>443.41334000000001</v>
       </c>
       <c r="D25">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>339.57481999999999</v>
+        <v>443.41334000000001</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>242</v>
       </c>
       <c r="C26">
-        <v>478.136503</v>
+        <v>422.29056200000002</v>
       </c>
       <c r="D26">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>303.18524100000002</v>
+        <v>422.29056200000002</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B27" t="s">
-        <v>259</v>
+        <v>27</v>
       </c>
       <c r="C27">
-        <v>398.66424000000001</v>
+        <v>487.14986299999998</v>
       </c>
       <c r="D27">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>398.66424000000001</v>
+        <v>312.19860099999994</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>336</v>
+        <v>255</v>
       </c>
       <c r="B28" t="s">
-        <v>259</v>
+        <v>27</v>
       </c>
       <c r="C28">
-        <v>396.648359999999</v>
+        <v>463.12516299999999</v>
       </c>
       <c r="D28">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>396.648359999999</v>
+        <v>288.173901</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>480</v>
+        <v>256</v>
       </c>
       <c r="B29" t="s">
-        <v>259</v>
+        <v>27</v>
       </c>
       <c r="C29">
-        <v>633.04128000000003</v>
+        <v>503.14926300000002</v>
       </c>
       <c r="D29">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>633.04128000000003</v>
+        <v>328.19800099999998</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>481</v>
+        <v>257</v>
       </c>
       <c r="B30" t="s">
-        <v>259</v>
+        <v>27</v>
       </c>
       <c r="C30">
-        <v>661.09443999999996</v>
+        <v>478.136503</v>
       </c>
       <c r="D30">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>661.09443999999996</v>
+        <v>303.18524100000002</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>337</v>
+        <v>230</v>
       </c>
       <c r="B31" t="s">
-        <v>334</v>
+        <v>41</v>
       </c>
       <c r="C31">
-        <v>65560.645239999998</v>
+        <v>424.177302</v>
       </c>
       <c r="D31">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>65560.645239999998</v>
+        <v>424.177302</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="B32" t="s">
-        <v>242</v>
+        <v>41</v>
       </c>
       <c r="C32">
-        <v>782.52592200000004</v>
+        <v>1.0079400000000001</v>
       </c>
       <c r="D32">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>782.52592200000004</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+        <v>1.0079400000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>276</v>
+        <v>231</v>
       </c>
       <c r="B33" t="s">
-        <v>274</v>
+        <v>41</v>
       </c>
       <c r="C33">
-        <v>55.844999999999999</v>
+        <v>18.015280000000001</v>
       </c>
       <c r="D33">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>55.844999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+        <v>18.015280000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>338</v>
+        <v>311</v>
       </c>
       <c r="B34" t="s">
-        <v>274</v>
+        <v>312</v>
       </c>
       <c r="C34">
-        <v>55.844999999999999</v>
+        <v>0</v>
       </c>
       <c r="D34">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>55.844999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>237</v>
+        <v>313</v>
       </c>
       <c r="B35" t="s">
-        <v>235</v>
+        <v>312</v>
       </c>
       <c r="C35">
-        <v>2619.1368040000002</v>
+        <v>0</v>
       </c>
       <c r="D35">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>2619.1368040000002</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>289</v>
+        <v>314</v>
       </c>
       <c r="B36" t="s">
-        <v>284</v>
+        <v>312</v>
       </c>
       <c r="C36">
-        <v>129.13715999999999</v>
+        <v>0</v>
       </c>
       <c r="D36">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>129.13715999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>290</v>
+        <v>315</v>
       </c>
       <c r="B37" t="s">
-        <v>284</v>
+        <v>312</v>
       </c>
       <c r="C37">
-        <v>129.11398</v>
+        <v>0</v>
       </c>
       <c r="D37">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>129.11398</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>339</v>
+        <v>316</v>
       </c>
       <c r="B38" t="s">
-        <v>235</v>
+        <v>312</v>
       </c>
       <c r="C38">
-        <v>162.14060000000001</v>
+        <v>0</v>
       </c>
       <c r="D38">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>162.14060000000001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>291</v>
+        <v>317</v>
       </c>
       <c r="B39" t="s">
-        <v>284</v>
+        <v>312</v>
       </c>
       <c r="C39">
-        <v>58.059260000000002</v>
+        <v>0</v>
       </c>
       <c r="D39">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>58.059260000000002</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>239</v>
+        <v>318</v>
       </c>
       <c r="B40" t="s">
-        <v>235</v>
+        <v>312</v>
       </c>
       <c r="C40">
-        <v>2280.41334042176</v>
+        <v>0</v>
       </c>
       <c r="D40">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>2280.41334042176</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>340</v>
+        <v>319</v>
       </c>
       <c r="B41" t="s">
-        <v>334</v>
+        <v>312</v>
       </c>
       <c r="C41">
-        <v>306.31554</v>
+        <v>0</v>
       </c>
       <c r="D41">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>306.31554</v>
-      </c>
-      <c r="E41" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="B42" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="C42">
-        <v>519.14866300000006</v>
+        <v>0</v>
       </c>
       <c r="D42">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>344.19740100000001</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>232</v>
+        <v>321</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>312</v>
       </c>
       <c r="C43">
-        <v>1.0079400000000001</v>
+        <v>0</v>
       </c>
       <c r="D43">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>1.0079400000000001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>312</v>
       </c>
       <c r="C44">
-        <v>18.015280000000001</v>
+        <v>0</v>
       </c>
       <c r="D44">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>18.015280000000001</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>261</v>
+        <v>323</v>
       </c>
       <c r="B45" t="s">
-        <v>259</v>
+        <v>312</v>
       </c>
       <c r="C45">
-        <v>255.41533999999999</v>
+        <v>0</v>
       </c>
       <c r="D45">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>255.41533999999999</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>482</v>
+        <v>324</v>
       </c>
       <c r="B46" t="s">
-        <v>259</v>
+        <v>312</v>
       </c>
       <c r="C46">
-        <v>253.39946</v>
+        <v>0</v>
       </c>
       <c r="D46">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>253.39946</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>246</v>
+        <v>325</v>
       </c>
       <c r="B47" t="s">
-        <v>242</v>
+        <v>312</v>
       </c>
       <c r="C47">
-        <v>850.82126000000005</v>
+        <v>0</v>
       </c>
       <c r="D47">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>850.82126000000005</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>292</v>
+        <v>326</v>
       </c>
       <c r="B48" t="s">
-        <v>284</v>
+        <v>312</v>
       </c>
       <c r="C48">
-        <v>138.14722</v>
+        <v>0</v>
       </c>
       <c r="D48">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>138.14722</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>293</v>
+        <v>327</v>
       </c>
       <c r="B49" t="s">
-        <v>284</v>
+        <v>312</v>
       </c>
       <c r="C49">
-        <v>114.16558000000001</v>
+        <v>0</v>
       </c>
       <c r="D49">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>114.16558000000001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>262</v>
+        <v>328</v>
       </c>
       <c r="B50" t="s">
-        <v>259</v>
+        <v>312</v>
       </c>
       <c r="C50">
-        <v>915.26344200000005</v>
+        <v>0</v>
       </c>
       <c r="D50">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>915.26344200000005</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>277</v>
+        <v>329</v>
       </c>
       <c r="B51" t="s">
-        <v>274</v>
+        <v>312</v>
       </c>
       <c r="C51">
-        <v>39.098300000000002</v>
+        <v>0</v>
       </c>
       <c r="D51">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>39.098300000000002</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>294</v>
+        <v>330</v>
       </c>
       <c r="B52" t="s">
-        <v>284</v>
+        <v>312</v>
       </c>
       <c r="C52">
-        <v>114.16558000000001</v>
+        <v>0</v>
       </c>
       <c r="D52">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>114.16558000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>263</v>
+        <v>331</v>
       </c>
       <c r="B53" t="s">
-        <v>259</v>
+        <v>312</v>
       </c>
       <c r="C53">
-        <v>279.43673999999999</v>
+        <v>0</v>
       </c>
       <c r="D53">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>279.43673999999999</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B54" t="s">
         <v>259</v>
       </c>
       <c r="C54">
-        <v>277.42086</v>
+        <v>339.57481999999999</v>
       </c>
       <c r="D54">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>277.42086</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+        <v>339.57481999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>295</v>
+        <v>260</v>
       </c>
       <c r="B55" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
       <c r="C55">
-        <v>130.18816000000001</v>
+        <v>398.66424000000001</v>
       </c>
       <c r="D55">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>130.18816000000001</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+        <v>398.66424000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="B56" t="s">
-        <v>235</v>
+        <v>259</v>
       </c>
       <c r="C56">
-        <v>162.14060000000001</v>
+        <v>396.648359999999</v>
       </c>
       <c r="D56">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>162.14060000000001</v>
-      </c>
-      <c r="E56" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+        <v>396.648359999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>296</v>
+        <v>480</v>
       </c>
       <c r="B57" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
       <c r="C57">
-        <v>132.20400000000001</v>
+        <v>633.04128000000003</v>
       </c>
       <c r="D57">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>132.20400000000001</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+        <v>633.04128000000003</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>278</v>
+        <v>481</v>
       </c>
       <c r="B58" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="C58">
-        <v>24.305</v>
+        <v>661.09443999999996</v>
       </c>
       <c r="D58">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>24.305</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+        <v>661.09443999999996</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
-        <v>343</v>
+        <v>261</v>
       </c>
       <c r="B59" t="s">
-        <v>334</v>
+        <v>259</v>
       </c>
       <c r="C59">
-        <v>455.42403999999999</v>
+        <v>255.41533999999999</v>
       </c>
       <c r="D59">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>455.42403999999999</v>
-      </c>
-      <c r="E59" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+        <v>255.41533999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>279</v>
+        <v>482</v>
       </c>
       <c r="B60" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="C60">
-        <v>54.938043999999998</v>
+        <v>253.39946</v>
       </c>
       <c r="D60">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>54.938043999999998</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+        <v>253.39946</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>344</v>
+        <v>262</v>
       </c>
       <c r="B61" t="s">
-        <v>334</v>
+        <v>259</v>
       </c>
       <c r="C61">
-        <v>22.98977</v>
+        <v>915.26344200000005</v>
       </c>
       <c r="D61">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>22.98977</v>
-      </c>
-      <c r="E61" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
+        <v>915.26344200000005</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="B62" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="C62">
-        <v>662.41716199999996</v>
+        <v>279.43673999999999</v>
       </c>
       <c r="D62">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>662.41716199999996</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
+        <v>279.43673999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
-        <v>479</v>
+        <v>264</v>
       </c>
       <c r="B63" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="C63">
-        <v>663.42510200000004</v>
+        <v>277.42086</v>
       </c>
       <c r="D63">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>663.42510200000004</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
+        <v>277.42086</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
-        <v>248</v>
+        <v>265</v>
       </c>
       <c r="B64" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="C64">
-        <v>740.38118299999996</v>
+        <v>283.46850000000001</v>
       </c>
       <c r="D64">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>740.38118299999996</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
+        <v>283.46850000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
-        <v>478</v>
+        <v>266</v>
       </c>
       <c r="B65" t="s">
-        <v>242</v>
-      </c>
-      <c r="C65" s="49">
-        <v>741.38912300000004</v>
+        <v>259</v>
+      </c>
+      <c r="C65">
+        <v>281.45262000000002</v>
       </c>
       <c r="D65">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>741.38912300000004</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+        <v>281.45262000000002</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B66" t="s">
         <v>259</v>
       </c>
       <c r="C66">
-        <v>283.46850000000001</v>
+        <v>862.14885442176001</v>
       </c>
       <c r="D66">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>283.46850000000001</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+        <v>862.14885442176001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B67" t="s">
         <v>259</v>
       </c>
       <c r="C67">
-        <v>281.45262000000002</v>
+        <v>786.16573442176002</v>
       </c>
       <c r="D67">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>281.45262000000002</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+        <v>786.16573442176002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
-        <v>240</v>
+        <v>269</v>
       </c>
       <c r="B68" t="s">
-        <v>235</v>
+        <v>259</v>
       </c>
       <c r="C68">
-        <v>810.70299999999997</v>
+        <v>744.08599442176001</v>
       </c>
       <c r="D68">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>810.70299999999997</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+        <v>744.08599442176001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
-        <v>345</v>
+        <v>270</v>
       </c>
       <c r="B69" t="s">
-        <v>334</v>
+        <v>259</v>
       </c>
       <c r="C69">
-        <v>69581.537779999999</v>
+        <v>786.07881442175994</v>
       </c>
       <c r="D69">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>69581.537779999999</v>
-      </c>
-      <c r="E69" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+        <v>786.07881442175994</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B70" t="s">
         <v>259</v>
       </c>
       <c r="C70">
-        <v>862.14885442176001</v>
+        <v>885.51292863263996</v>
       </c>
       <c r="D70">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>862.14885442176001</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+        <v>885.51292863263996</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B71" t="s">
         <v>259</v>
       </c>
       <c r="C71">
-        <v>786.16573442176002</v>
+        <v>367.62797999999998</v>
       </c>
       <c r="D71">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>786.16573442176002</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+        <v>367.62797999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B72" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="C72">
-        <v>744.08599442176001</v>
+        <v>40.078000000000003</v>
       </c>
       <c r="D72">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>744.08599442176001</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+        <v>40.078000000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
-        <v>297</v>
+        <v>275</v>
       </c>
       <c r="B73" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C73">
-        <v>148.18180000000001</v>
+        <v>63.545999999999999</v>
       </c>
       <c r="D73">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>148.18180000000001</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
+        <v>63.545999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B74" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C74">
-        <v>95.979301000000007</v>
+        <v>55.844999999999999</v>
       </c>
       <c r="D74">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>95.979301000000007</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
+        <v>55.844999999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
-        <v>233</v>
+        <v>338</v>
+      </c>
+      <c r="B75" t="s">
+        <v>274</v>
       </c>
       <c r="C75">
-        <v>174.95126200000001</v>
+        <v>55.844999999999999</v>
       </c>
       <c r="D75">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>174.95126200000001</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
+        <v>55.844999999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
-        <v>298</v>
+        <v>277</v>
       </c>
       <c r="B76" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C76">
-        <v>97.115179999999995</v>
+        <v>39.098300000000002</v>
       </c>
       <c r="D76">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>97.115179999999995</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
+        <v>39.098300000000002</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="B77" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="C77">
-        <v>786.07881442175994</v>
+        <v>24.305</v>
       </c>
       <c r="D77">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>786.07881442175994</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
+        <v>24.305</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
-        <v>346</v>
+        <v>279</v>
       </c>
       <c r="B78" t="s">
-        <v>334</v>
+        <v>274</v>
       </c>
       <c r="C78">
-        <v>318.51510000000002</v>
+        <v>54.938043999999998</v>
       </c>
       <c r="D78">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>318.51510000000002</v>
-      </c>
-      <c r="E78" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
+        <v>54.938043999999998</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
-        <v>347</v>
+        <v>280</v>
       </c>
       <c r="B79" t="s">
-        <v>334</v>
+        <v>274</v>
       </c>
       <c r="C79">
-        <v>90.167360000000002</v>
+        <v>65.38</v>
       </c>
       <c r="D79">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>90.167360000000002</v>
-      </c>
-      <c r="E79" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
+        <v>65.38</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
-        <v>249</v>
+        <v>333</v>
       </c>
       <c r="B80" t="s">
-        <v>242</v>
+        <v>334</v>
       </c>
       <c r="C80">
-        <v>245.126</v>
+        <v>328.19800099999998</v>
       </c>
       <c r="D80">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>245.126</v>
+        <v>328.19800099999998</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
       <c r="B81" t="s">
         <v>334</v>
       </c>
       <c r="C81">
-        <v>795.22648000000004</v>
+        <v>144970.98955999999</v>
       </c>
       <c r="D81">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>795.22648000000004</v>
-      </c>
-      <c r="E81" t="s">
-        <v>341</v>
+        <v>144970.98955999999</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
-        <v>250</v>
+        <v>337</v>
       </c>
       <c r="B82" t="s">
-        <v>242</v>
+        <v>334</v>
       </c>
       <c r="C82">
-        <v>375.35595999999998</v>
+        <v>65560.645239999998</v>
       </c>
       <c r="D82">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>375.35595999999998</v>
+        <v>65560.645239999998</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
-        <v>299</v>
+        <v>340</v>
       </c>
       <c r="B83" t="s">
-        <v>284</v>
+        <v>334</v>
       </c>
       <c r="C83">
-        <v>88.085239999999999</v>
+        <v>306.31554</v>
       </c>
       <c r="D83">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>88.085239999999999</v>
+        <v>306.31554</v>
+      </c>
+      <c r="E83" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
-        <v>309</v>
+        <v>343</v>
       </c>
       <c r="B84" t="s">
-        <v>310</v>
+        <v>334</v>
       </c>
       <c r="C84">
-        <v>96.062600000000003</v>
+        <v>455.42403999999999</v>
       </c>
       <c r="D84">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>96.062600000000003</v>
+        <v>455.42403999999999</v>
+      </c>
+      <c r="E84" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
-        <v>251</v>
+        <v>344</v>
       </c>
       <c r="B85" t="s">
-        <v>242</v>
+        <v>334</v>
       </c>
       <c r="C85">
-        <v>148.26967999999999</v>
+        <v>22.98977</v>
       </c>
       <c r="D85">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>148.26967999999999</v>
+        <v>22.98977</v>
+      </c>
+      <c r="E85" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
-        <v>271</v>
+        <v>345</v>
       </c>
       <c r="B86" t="s">
-        <v>259</v>
+        <v>334</v>
       </c>
       <c r="C86">
-        <v>885.51292863263996</v>
+        <v>69581.537779999999</v>
       </c>
       <c r="D86">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>885.51292863263996</v>
+        <v>69581.537779999999</v>
+      </c>
+      <c r="E86" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
-        <v>252</v>
+        <v>346</v>
       </c>
       <c r="B87" t="s">
-        <v>242</v>
+        <v>334</v>
       </c>
       <c r="C87">
-        <v>443.41334000000001</v>
+        <v>318.51510000000002</v>
       </c>
       <c r="D87">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>443.41334000000001</v>
+        <v>318.51510000000002</v>
+      </c>
+      <c r="E87" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
-        <v>253</v>
+        <v>347</v>
       </c>
       <c r="B88" t="s">
-        <v>242</v>
+        <v>334</v>
       </c>
       <c r="C88">
-        <v>422.29056200000002</v>
+        <v>90.167360000000002</v>
       </c>
       <c r="D88">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>422.29056200000002</v>
+        <v>90.167360000000002</v>
+      </c>
+      <c r="E88" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
-        <v>300</v>
+        <v>348</v>
       </c>
       <c r="B89" t="s">
-        <v>284</v>
+        <v>334</v>
       </c>
       <c r="C89">
-        <v>102.11181999999999</v>
+        <v>795.22648000000004</v>
       </c>
       <c r="D89">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>102.11181999999999</v>
+        <v>795.22648000000004</v>
+      </c>
+      <c r="E89" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B90" t="s">
-        <v>235</v>
+        <v>334</v>
       </c>
       <c r="C90">
-        <v>342.29647999999997</v>
+        <v>384.63765999999998</v>
       </c>
       <c r="D90">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>342.29647999999997</v>
+        <v>384.63765999999998</v>
       </c>
       <c r="E90" t="s">
         <v>341</v>
@@ -14172,428 +14178,422 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
-        <v>311</v>
+        <v>351</v>
       </c>
       <c r="B91" t="s">
-        <v>312</v>
+        <v>334</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>64359.575239999998</v>
       </c>
       <c r="D91">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>64359.575239999998</v>
+      </c>
+      <c r="E91" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="B92" t="s">
-        <v>312</v>
+        <v>282</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>95.979301000000007</v>
       </c>
       <c r="D92">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>95.979301000000007</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>314</v>
+        <v>283</v>
       </c>
       <c r="B93" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>72.085840000000005</v>
       </c>
       <c r="D93">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>72.085840000000005</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
-        <v>315</v>
+        <v>285</v>
       </c>
       <c r="B94" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>158.20156</v>
       </c>
       <c r="D94">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>158.20156</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
-        <v>316</v>
+        <v>286</v>
       </c>
       <c r="B95" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>115.11058</v>
       </c>
       <c r="D95">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>115.11058</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
-        <v>317</v>
+        <v>287</v>
       </c>
       <c r="B96" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C96">
-        <v>0</v>
+        <v>115.0874</v>
       </c>
       <c r="D96">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>115.0874</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
-        <v>318</v>
+        <v>288</v>
       </c>
       <c r="B97" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C97">
-        <v>0</v>
+        <v>104.15084</v>
       </c>
       <c r="D97">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>104.15084</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
-        <v>319</v>
+        <v>289</v>
       </c>
       <c r="B98" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>129.13715999999999</v>
       </c>
       <c r="D98">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>129.13715999999999</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
-        <v>320</v>
+        <v>290</v>
       </c>
       <c r="B99" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>129.11398</v>
       </c>
       <c r="D99">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>129.11398</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
-        <v>321</v>
+        <v>291</v>
       </c>
       <c r="B100" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>58.059260000000002</v>
       </c>
       <c r="D100">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>58.059260000000002</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
-        <v>322</v>
+        <v>292</v>
       </c>
       <c r="B101" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>138.14722</v>
       </c>
       <c r="D101">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>138.14722</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
-        <v>323</v>
+        <v>293</v>
       </c>
       <c r="B102" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C102">
-        <v>0</v>
+        <v>114.16558000000001</v>
       </c>
       <c r="D102">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>114.16558000000001</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
-        <v>324</v>
+        <v>294</v>
       </c>
       <c r="B103" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>114.16558000000001</v>
       </c>
       <c r="D103">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>114.16558000000001</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
       <c r="B104" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C104">
-        <v>0</v>
+        <v>130.18816000000001</v>
       </c>
       <c r="D104">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>130.18816000000001</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
-        <v>326</v>
+        <v>296</v>
       </c>
       <c r="B105" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>132.20400000000001</v>
       </c>
       <c r="D105">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>132.20400000000001</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
-        <v>327</v>
+        <v>297</v>
       </c>
       <c r="B106" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>148.18180000000001</v>
       </c>
       <c r="D106">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>148.18180000000001</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
-        <v>328</v>
+        <v>298</v>
       </c>
       <c r="B107" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>97.115179999999995</v>
       </c>
       <c r="D107">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>97.115179999999995</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
-        <v>329</v>
+        <v>299</v>
       </c>
       <c r="B108" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>88.085239999999999</v>
       </c>
       <c r="D108">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>88.085239999999999</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
-        <v>330</v>
+        <v>300</v>
       </c>
       <c r="B109" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>102.11181999999999</v>
       </c>
       <c r="D109">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>102.11181999999999</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
-        <v>331</v>
+        <v>301</v>
       </c>
       <c r="B110" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>187.21784</v>
       </c>
       <c r="D110">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>0</v>
+        <v>187.21784</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B111" t="s">
         <v>284</v>
       </c>
       <c r="C111">
-        <v>187.21784</v>
+        <v>164.18119999999999</v>
       </c>
       <c r="D111">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>187.21784</v>
+        <v>164.18119999999999</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
-        <v>272</v>
+        <v>303</v>
       </c>
       <c r="B112" t="s">
-        <v>259</v>
+        <v>284</v>
       </c>
       <c r="C112">
-        <v>367.62797999999998</v>
+        <v>100.139</v>
       </c>
       <c r="D112">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>367.62797999999998</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.15">
+        <v>100.139</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B113" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="C113">
-        <v>164.18119999999999</v>
+        <v>503.14926300000002</v>
       </c>
       <c r="D113">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>164.18119999999999</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.15">
+        <v>328.19800099999998</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B114" t="s">
         <v>305</v>
       </c>
       <c r="C114">
-        <v>480.10932300000002</v>
+        <v>479.12456300000002</v>
       </c>
       <c r="D114">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>305.15806099999998</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.15">
+        <v>304.17330100000004</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="B115" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="C115">
-        <v>100.139</v>
+        <v>519.14866300000006</v>
       </c>
       <c r="D115">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>100.139</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.15">
+        <v>344.19740100000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
-        <v>280</v>
+        <v>308</v>
       </c>
       <c r="B116" t="s">
-        <v>274</v>
+        <v>305</v>
       </c>
       <c r="C116">
-        <v>65.38</v>
+        <v>480.10932300000002</v>
       </c>
       <c r="D116">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>65.38</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.15">
+        <v>305.15806099999998</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
-        <v>350</v>
+        <v>309</v>
       </c>
       <c r="B117" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="C117">
-        <v>384.63765999999998</v>
+        <v>96.062600000000003</v>
       </c>
       <c r="D117">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>384.63765999999998</v>
-      </c>
-      <c r="E117" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.15">
+        <v>96.062600000000003</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
-        <v>351</v>
-      </c>
-      <c r="B118" t="s">
-        <v>334</v>
+        <v>233</v>
       </c>
       <c r="C118">
-        <v>64359.575239999998</v>
+        <v>174.95126200000001</v>
       </c>
       <c r="D118">
         <f>IF(IFERROR(MATCH(metaboliteInfo[[#This Row],[name w/o location]],{"atp","ctp","gtp","utp","datp","dctp","dgtp","dttp"},0),0)&gt;0,metaboliteInfo[[#This Row],[MW (g/mol)]]-174.951262,metaboliteInfo[[#This Row],[MW (g/mol)]])</f>
-        <v>64359.575239999998</v>
-      </c>
-      <c r="E118" t="s">
-        <v>341</v>
+        <v>174.95126200000001</v>
       </c>
     </row>
   </sheetData>
@@ -14612,7 +14612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5455B0F7-CD7B-1440-98EA-12626AC5D91D}">
   <dimension ref="A1:K111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
biomass updates finally committed, NGAM enforced
</commit_message>
<xml_diff>
--- a/build_model/input/BIOMASS_RBA.xlsx
+++ b/build_model/input/BIOMASS_RBA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejm6426/Documents/scRBA/build_model/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDE142A-74B0-0643-A0C9-57302C8598C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD708837-2EC1-C445-A313-43806BA858C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19640" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19640" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RBABioRxns" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="586">
   <si>
     <t>rxn_id</t>
   </si>
@@ -6005,6 +6005,41 @@
   </si>
   <si>
     <t>biomass equation from MFA results:</t>
+  </si>
+  <si>
+    <r>
+      <t>"ipc_g"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF098658"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>-0.003830</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <t>carb</t>
   </si>
 </sst>
 </file>
@@ -6320,7 +6355,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -6494,6 +6529,9 @@
     <xf numFmtId="0" fontId="13" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -7571,7 +7609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A27" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
@@ -8300,8 +8338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F168A7-6B4E-494D-BA75-6693E50B2433}">
   <dimension ref="A1:AG95"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="O1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15386,8 +15424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE6FF3F-114A-7C40-948C-4CCE76A11B92}">
   <dimension ref="A1:AG62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P38" sqref="P38:P57"/>
+    <sheetView topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15492,7 +15530,7 @@
       </c>
       <c r="T2" s="60">
         <f>0.391*SUM(T6,T12:T13)</f>
-        <v>7.5341019728080508E-2</v>
+        <v>7.5702317689710544E-2</v>
       </c>
       <c r="U2" s="60"/>
       <c r="V2" s="61" t="s">
@@ -15513,15 +15551,15 @@
       </c>
       <c r="G3" cm="1">
         <f t="array" ref="G3">_xlfn.LET(_xlpm.coeffs,mets27138[coeff. w/o GAM],-SUM(_xlfn._xlws.FILTER(_xlpm.coeffs*mets27138[MW for biomass normalization (g/mol)],(IFERROR(_xlfn.NUMBERVALUE(_xlpm.coeffs),0)&lt;0)*(_xlfn.IFNA(mets27138[category],"ignore")&lt;&gt;"ignore")))/1000)</f>
-        <v>2.9698864220227361</v>
+        <v>2.9733918810055959</v>
       </c>
       <c r="H3" s="60" cm="1">
         <f t="array" ref="H3">_xlfn.LET(_xlpm.coeffs,mets27138[coeffs after extra operations],-SUM(_xlfn._xlws.FILTER(_xlpm.coeffs*mets27138[MW for biomass normalization (g/mol)],(IFERROR(_xlfn.NUMBERVALUE(_xlpm.coeffs),0)&lt;0)*(_xlfn.IFNA(mets27138[category],"ignore")&lt;&gt;"ignore")))/1000)</f>
-        <v>2.9698864220227361</v>
+        <v>2.9733918810055959</v>
       </c>
       <c r="I3" s="57" cm="1">
         <f t="array" ref="I3">_xlfn.LET(_xlpm.coeffs,mets27138[normalized coeffs],-SUM(_xlfn._xlws.FILTER(_xlpm.coeffs*mets27138[MW for biomass normalization (g/mol)],(IFERROR(_xlfn.NUMBERVALUE(_xlpm.coeffs),0)&lt;0)*(_xlfn.IFNA(mets27138[category],"ignore")&lt;&gt;"ignore")))/1000)</f>
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="J3" s="60"/>
       <c r="L3" s="60"/>
@@ -15702,11 +15740,11 @@
       </c>
       <c r="I6" s="72">
         <f>H6/($H$3)</f>
-        <v>1.726915198496684</v>
+        <v>1.7248792642379411</v>
       </c>
       <c r="J6" s="37" cm="1">
         <f t="array" ref="J6">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>1.726915198496684</v>
+        <v>1.7248792642379411</v>
       </c>
       <c r="K6" t="str" cm="1">
         <f t="array" ref="K6">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -15718,7 +15756,7 @@
       </c>
       <c r="M6" s="73" cm="1">
         <f t="array" ref="M6">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>1.7242617250793584</v>
+        <v>1.7222381140492926</v>
       </c>
       <c r="N6" s="73"/>
       <c r="O6" s="74" t="str" cm="1">
@@ -15742,7 +15780,7 @@
       </c>
       <c r="T6" s="76" cm="1">
         <f t="array" ref="T6">IF(biomassComponents26127[[#This Row],[pre-determined coeffs]]&lt;&gt;"",biomassComponents26127[[#This Row],[pre-determined coeffs]]*IF(SUM(biomassComponents26127[pre-determined coeffs])&gt;1,1/SUM(biomassComponents26127[pre-determined coeffs]),1)*(1-SUM(_xlfn._xlws.FILTER(biomassComponents26127[original coeffs from input],biomassComponents26127[pre-determined coeffs]=""))),biomassComponents26127[[#This Row],[original coeffs from input]])</f>
-        <v>6.1185328855125169E-2</v>
+        <v>6.147874318209879E-2</v>
       </c>
       <c r="U6" s="75" t="e" cm="1">
         <f t="array" ref="U6">_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER(ROUND(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]*(biomassComponents26127[[#This Row],[normalized coeffs]]/biomassComponents26127[[#This Row],[original coeffs from input]])/(1000*biomassComponents26127[[#This Row],[normalized coeffs]]),6)&amp;" BIO-"&amp;mets27138[name],mets27138[category]=_xlfn.TEXTAFTER(O6,"BIOSYN-"),""))&amp;" --&gt; "&amp;biomassComponents26127[[#This Row],[product name]]</f>
@@ -15757,7 +15795,7 @@
       </c>
       <c r="Z6" t="str">
         <f>SUBSTITUTE(Z7," --&gt; "," + "&amp;K2)</f>
-        <v>0.192688029995091 BIO-varbiom + 0.0804139023515599 BIO-carb + 0.000503949450244104 BIO-dna + 0.00413898220441537 BIO-lipid + 0.00853626099306161 BIO-metal + 0.149625268542784 BIO-other + 0.564093606462844 BIO-rna + 128.722942 MET-h2o_c + 128.722942 MET-atp_c --&gt; 128.722942 MET-adp_c + 128.722942 MET-h_c + 128.722942 MET-pi_c</v>
+        <v>0.193612065702585 BIO-varbiom + 0.0803190989594656 BIO-carb + 0.000506366140511835 BIO-dna + 0.00415883069915403 BIO-lipid + 0.00852619722952969 BIO-metal + 0.149448868908068 BIO-other + 0.563428572360686 BIO-rna + 128.722942 MET-h2o_c + 128.722942 MET-atp_c --&gt; 128.722942 MET-adp_c + 128.722942 MET-h_c + 128.722942 MET-pi_c</v>
       </c>
       <c r="AB6" t="s">
         <v>2</v>
@@ -15768,23 +15806,23 @@
     </row>
     <row r="7" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="99" t="s">
-        <v>561</v>
+        <v>584</v>
       </c>
       <c r="B7" t="str">
         <f>SUBSTITUTE(_xlfn.TEXTBEFORE(mets27138[[#This Row],[pasted JSON metabolite keys and values from GSM biomass rxn]],":"),CHAR(34),"")</f>
-        <v>ipcbiom_c</v>
+        <v>ipc_g</v>
       </c>
       <c r="C7" t="str">
         <f>_xlfn.TEXTBEFORE(mets27138[[#This Row],[name]],"_",-1)</f>
-        <v>ipcbiom</v>
+        <v>ipc</v>
       </c>
       <c r="D7" t="str">
         <f>_xlfn.XLOOKUP(mets27138[[#This Row],[name w/o location]],metaboliteInfo[name w/o location],metaboliteInfo[suggested category],"")</f>
-        <v/>
+        <v>LIPID</v>
       </c>
       <c r="E7" s="37">
         <f>_xlfn.XLOOKUP(mets27138[[#This Row],[name w/o location]],metaboliteInfo[name w/o location],metaboliteInfo[MW for biomass normalization (g/mol)],0)</f>
-        <v>0</v>
+        <v>915.26344200000005</v>
       </c>
       <c r="F7" s="37">
         <f>_xlfn.NUMBERVALUE(SUBSTITUTE(_xlfn.TEXTAFTER(mets27138[[#This Row],[pasted JSON metabolite keys and values from GSM biomass rxn]],":"),",",""))</f>
@@ -15800,23 +15838,23 @@
       </c>
       <c r="I7" s="72">
         <f>H7/($H$3)</f>
-        <v>-1.2896116065581578E-3</v>
+        <v>-1.2880912282254235E-3</v>
       </c>
       <c r="J7" s="37" cm="1">
         <f t="array" ref="J7">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-1.2896116065581578E-3</v>
+        <v>-1.2880912282254235E-3</v>
       </c>
       <c r="K7" t="str" cm="1">
         <f t="array" ref="K7">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
-        <v>BIOSYN-ipcbiom_c</v>
+        <v>BIOSYN-LIPID-ipc_g</v>
       </c>
       <c r="L7" s="73" t="str" cm="1">
         <f t="array" ref="L7">IF(IsElementOfSet_DIY(mets27138[[#This Row],[category]],{"ignore","PROT"}),"",_xlfn.LET(_xlpm.mw,mets27138[[#This Row],[MW for biomass normalization (g/mol)]],"MET-"&amp;mets27138[[#This Row],[name]]&amp;" --&gt; "&amp;IF((mets27138[[#This Row],[category]]="DNA")+(mets27138[[#This Row],[category]]="RNA"),"MET-ppi_c + ","")&amp;ROUND(ABS(_xlpm.mw/1000),6)&amp;" BIO-"&amp;mets27138[[#This Row],[name]]))</f>
-        <v>MET-ipcbiom_c --&gt; 0 BIO-ipcbiom_c</v>
-      </c>
-      <c r="M7" s="73" t="e" cm="1">
+        <v>MET-ipc_g --&gt; 0.915263 BIO-ipc_g</v>
+      </c>
+      <c r="M7" s="73" cm="1">
         <f t="array" ref="M7">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>#DIV/0!</v>
+        <v>-2.8459495336420734E-4</v>
       </c>
       <c r="N7" s="73"/>
       <c r="O7" s="74" t="str">
@@ -15832,12 +15870,12 @@
       </c>
       <c r="R7" s="76" cm="1">
         <f t="array" ref="R7">SUM(_xlfn._xlws.FILTER(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]/1000,mets27138[category]=_xlfn.TEXTAFTER(O7,"BIOSYN-"),""))</f>
-        <v>8.0413902351559929E-2</v>
+        <v>8.031909895946561E-2</v>
       </c>
       <c r="S7" s="83"/>
       <c r="T7" s="76" cm="1">
         <f t="array" ref="T7">IF(biomassComponents26127[[#This Row],[pre-determined coeffs]]&lt;&gt;"",biomassComponents26127[[#This Row],[pre-determined coeffs]]*IF(SUM(biomassComponents26127[pre-determined coeffs])&gt;1,1/SUM(biomassComponents26127[pre-determined coeffs]),1)*(1-SUM(_xlfn._xlws.FILTER(biomassComponents26127[original coeffs from input],biomassComponents26127[pre-determined coeffs]=""))),biomassComponents26127[[#This Row],[original coeffs from input]])</f>
-        <v>8.0413902351559929E-2</v>
+        <v>8.031909895946561E-2</v>
       </c>
       <c r="U7" s="75" t="str" cm="1">
         <f t="array" ref="U7">_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER(ROUND(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]*(biomassComponents26127[[#This Row],[normalized coeffs]]/biomassComponents26127[[#This Row],[original coeffs from input]])/(1000*biomassComponents26127[[#This Row],[normalized coeffs]]),6)&amp;" BIO-"&amp;mets27138[name],mets27138[category]=_xlfn.TEXTAFTER(O7,"BIOSYN-"),""))&amp;" --&gt; "&amp;biomassComponents26127[[#This Row],[product name]]</f>
@@ -15845,7 +15883,7 @@
       </c>
       <c r="V7" s="75" t="str" cm="1">
         <f t="array" ref="V7">_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER((-mets27138[normalized coeffs]*biomassComponents26127[[#This Row],[normalized coeffs]]/biomassComponents26127[[#This Row],[original coeffs from input]])&amp;" BIO-"&amp;mets27138[name],mets27138[category]=_xlfn.TEXTAFTER(P7,"BIOSYN-"),""))</f>
-        <v>0.129375317908052 BIO-mannan_c + 0.20076255966513 BIO-13BDglucan_c + 0.0528323234304476 BIO-16BDglucan_c + 0.00474664616648834 BIO-chtn_c + 0.0967905701269944 BIO-glycogen_c + 0.00485170068900692 BIO-tre_c</v>
+        <v>0.129222791807064 BIO-mannan_c + 0.200525872088664 BIO-13BDglucan_c + 0.0527700371425426 BIO-16BDglucan_c + 0.00474105014211326 BIO-chtn_c + 0.0966764595801555 BIO-glycogen_c + 0.00484598081135774 BIO-tre_c</v>
       </c>
       <c r="Y7" s="77" t="str">
         <f>Y6&amp;"-NOGAM"</f>
@@ -15853,7 +15891,7 @@
       </c>
       <c r="Z7" t="str" cm="1">
         <f t="array" ref="Z7">_xlfn.LET(_xlpm.varbiom,_xlfn.HSTACK(_xlfn.VSTACK(Q6,Q12:Q13),_xlfn.VSTACK(T6,T12:T13)),_xlpm.non_varbiom,IFERROR(_xlfn.XLOOKUP(biomassComponents26127[product name],_xlfn.CHOOSECOLS(_xlpm.varbiom,1),LEFT(_xlfn.CHOOSECOLS(_xlpm.varbiom,1),0),biomassComponents26127[product name]),_xlfn.HSTACK(biomassComponents26127[product name],biomassComponents26127[normalized coeffs])),_xlpm.old,_xlfn.TEXTJOIN(" + ",TRUE,SUM(_xlfn.CHOOSECOLS(_xlpm.varbiom,2))&amp;" BIO-varbiom",_xlfn._xlws.FILTER(_xlfn.CHOOSECOLS(_xlpm.non_varbiom,2)&amp;" "&amp;_xlfn.CHOOSECOLS(_xlpm.non_varbiom,1),(_xlfn.NUMBERVALUE(_xlfn.CHOOSECOLS(_xlpm.non_varbiom,2))&lt;&gt;0)))&amp;" --&gt; ",_xlpm.old)</f>
-        <v xml:space="preserve">0.192688029995091 BIO-varbiom + 0.0804139023515599 BIO-carb + 0.000503949450244104 BIO-dna + 0.00413898220441537 BIO-lipid + 0.00853626099306161 BIO-metal + 0.149625268542784 BIO-other + 0.564093606462844 BIO-rna --&gt; </v>
+        <v xml:space="preserve">0.193612065702585 BIO-varbiom + 0.0803190989594656 BIO-carb + 0.000506366140511835 BIO-dna + 0.00415883069915403 BIO-lipid + 0.00852619722952969 BIO-metal + 0.149448868908068 BIO-other + 0.563428572360686 BIO-rna --&gt; </v>
       </c>
       <c r="AB7" t="s">
         <v>4</v>
@@ -15896,11 +15934,11 @@
       </c>
       <c r="I8" s="72">
         <f>H8/($H$3)</f>
-        <v>-4.9631527625763048E-4</v>
+        <v>-4.957301489306199E-4</v>
       </c>
       <c r="J8" s="37" cm="1">
         <f t="array" ref="J8">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-4.9631527625763048E-4</v>
+        <v>-4.957301489306199E-4</v>
       </c>
       <c r="K8" t="str" cm="1">
         <f t="array" ref="K8">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -15928,14 +15966,14 @@
       </c>
       <c r="R8" s="76" cm="1">
         <f t="array" ref="R8">SUM(_xlfn._xlws.FILTER(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]/1000,mets27138[category]=_xlfn.TEXTAFTER(O8,"BIOSYN-"),""))</f>
-        <v>1.372810937054342E-3</v>
+        <v>1.3711924714690262E-3</v>
       </c>
       <c r="S8" s="84">
         <v>0.25538285833653501</v>
       </c>
       <c r="T8" s="76" cm="1">
         <f t="array" ref="T8">IF(biomassComponents26127[[#This Row],[pre-determined coeffs]]&lt;&gt;"",biomassComponents26127[[#This Row],[pre-determined coeffs]]*IF(SUM(biomassComponents26127[pre-determined coeffs])&gt;1,1/SUM(biomassComponents26127[pre-determined coeffs]),1)*(1-SUM(_xlfn._xlws.FILTER(biomassComponents26127[original coeffs from input],biomassComponents26127[pre-determined coeffs]=""))),biomassComponents26127[[#This Row],[original coeffs from input]])</f>
-        <v>5.0394945024410389E-4</v>
+        <v>5.0636614051183487E-4</v>
       </c>
       <c r="U8" s="75" t="str" cm="1">
         <f t="array" ref="U8">_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER(ROUND(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]*(biomassComponents26127[[#This Row],[normalized coeffs]]/biomassComponents26127[[#This Row],[original coeffs from input]])/(1000*biomassComponents26127[[#This Row],[normalized coeffs]]),6)&amp;" BIO-"&amp;mets27138[name],mets27138[category]=_xlfn.TEXTAFTER(O8,"BIOSYN-"),""))&amp;" --&gt; "&amp;biomassComponents26127[[#This Row],[product name]]</f>
@@ -15943,7 +15981,7 @@
       </c>
       <c r="V8" s="75" t="str" cm="1">
         <f t="array" ref="V8">_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER((-mets27138[normalized coeffs]*biomassComponents26127[[#This Row],[normalized coeffs]]/biomassComponents26127[[#This Row],[original coeffs from input]])&amp;" BIO-"&amp;mets27138[name],mets27138[category]=_xlfn.TEXTAFTER(P8,"BIOSYN-"),""))</f>
-        <v>0.000488610976213964 BIO-datp_c + 0.000329778417540818 BIO-dctp_c + 0.000329778417540818 BIO-dgtp_c + 0.000488610976213964 BIO-dttp_c</v>
+        <v>0.000490954110808814 BIO-datp_c + 0.000331359870386521 BIO-dctp_c + 0.000331359870386521 BIO-dgtp_c + 0.000490954110808814 BIO-dttp_c</v>
       </c>
       <c r="X8" s="78" t="s">
         <v>384</v>
@@ -15995,11 +16033,11 @@
       </c>
       <c r="I9" s="72">
         <f>H9/($H$3)</f>
-        <v>1.5836299210381031</v>
+        <v>1.5817629119271643</v>
       </c>
       <c r="J9" s="37" cm="1">
         <f t="array" ref="J9">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>1.5836299210381031</v>
+        <v>1.5817629119271643</v>
       </c>
       <c r="K9" t="str" cm="1">
         <f t="array" ref="K9">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -16027,22 +16065,22 @@
       </c>
       <c r="R9" s="76" cm="1">
         <f t="array" ref="R9">SUM(_xlfn._xlws.FILTER(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]/1000,mets27138[category]=_xlfn.TEXTAFTER(O9,"BIOSYN-"),""))</f>
-        <v>1.7664962355730614E-2</v>
+        <v>1.8823079186507601E-2</v>
       </c>
       <c r="S9" s="83">
         <v>2.0974824071256464</v>
       </c>
       <c r="T9" s="76" cm="1">
         <f t="array" ref="T9">IF(biomassComponents26127[[#This Row],[pre-determined coeffs]]&lt;&gt;"",biomassComponents26127[[#This Row],[pre-determined coeffs]]*IF(SUM(biomassComponents26127[pre-determined coeffs])&gt;1,1/SUM(biomassComponents26127[pre-determined coeffs]),1)*(1-SUM(_xlfn._xlws.FILTER(biomassComponents26127[original coeffs from input],biomassComponents26127[pre-determined coeffs]=""))),biomassComponents26127[[#This Row],[original coeffs from input]])</f>
-        <v>4.1389822044153677E-3</v>
+        <v>4.1588306991540312E-3</v>
       </c>
       <c r="U9" s="75" t="str" cm="1">
         <f t="array" ref="U9">_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER(ROUND(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]*(biomassComponents26127[[#This Row],[normalized coeffs]]/biomassComponents26127[[#This Row],[original coeffs from input]])/(1000*biomassComponents26127[[#This Row],[normalized coeffs]]),6)&amp;" BIO-"&amp;mets27138[name],mets27138[category]=_xlfn.TEXTAFTER(O9,"BIOSYN-"),""))&amp;" --&gt; "&amp;biomassComponents26127[[#This Row],[product name]]</f>
-        <v>0.200165 BIO-ergst_c + 0.113095 BIO-pail_c + 0.384789 BIO-pc_c + 0.097877 BIO-pe_c + 0.088807 BIO-ps_c + 0.115266 BIO-tag_c --&gt; BIO-lipid</v>
+        <v>0.062633 BIO-ipc_g + 0.187629 BIO-ergst_c + 0.106012 BIO-pail_c + 0.360689 BIO-pc_c + 0.091747 BIO-pe_c + 0.083245 BIO-ps_c + 0.108046 BIO-tag_c --&gt; BIO-lipid</v>
       </c>
       <c r="V9" s="75" t="str" cm="1">
         <f t="array" ref="V9">_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER((-mets27138[normalized coeffs]*biomassComponents26127[[#This Row],[normalized coeffs]]/biomassComponents26127[[#This Row],[original coeffs from input]])&amp;" BIO-"&amp;mets27138[name],mets27138[category]=_xlfn.TEXTAFTER(P9,"BIOSYN-"),""))</f>
-        <v>0.00208870434812752 BIO-ergst_c + 0.00054294479032346 BIO-pail_c + 0.00202582626066925 BIO-pc_c + 0.000544443766059604 BIO-pe_c + 0.000467601536217254 BIO-ps_c + 0.000538763436954215 BIO-tag_c</v>
+        <v>0.000284594953364207 BIO-ipc_g + 0.00196727190347713 BIO-ergst_c + 0.00051137923473955 BIO-pail_c + 0.00190804940273789 BIO-pc_c + 0.00051279106348992 BIO-pe_c + 0.000440416263339336 BIO-ps_c + 0.000507440975593779 BIO-tag_c</v>
       </c>
       <c r="X9" s="78"/>
       <c r="Y9" t="s">
@@ -16092,11 +16130,11 @@
       </c>
       <c r="I10" s="72">
         <f>H10/($H$3)</f>
-        <v>-0.12937531790805248</v>
+        <v>-0.12922279180706384</v>
       </c>
       <c r="J10" s="37" cm="1">
         <f t="array" ref="J10">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-0.12937531790805248</v>
+        <v>-0.12922279180706384</v>
       </c>
       <c r="K10" t="str" cm="1">
         <f t="array" ref="K10">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -16108,7 +16146,7 @@
       </c>
       <c r="M10" s="73" cm="1">
         <f t="array" ref="M10">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-0.12937531790805248</v>
+        <v>-0.12922279180706384</v>
       </c>
       <c r="N10" s="73"/>
       <c r="O10" s="74" t="str">
@@ -16124,12 +16162,12 @@
       </c>
       <c r="R10" s="76" cm="1">
         <f t="array" ref="R10">SUM(_xlfn._xlws.FILTER(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]/1000,mets27138[category]=_xlfn.TEXTAFTER(O10,"BIOSYN-"),""))</f>
-        <v>8.5362609930616125E-3</v>
+        <v>8.5261972295296931E-3</v>
       </c>
       <c r="S10" s="76"/>
       <c r="T10" s="76" cm="1">
         <f t="array" ref="T10">IF(biomassComponents26127[[#This Row],[pre-determined coeffs]]&lt;&gt;"",biomassComponents26127[[#This Row],[pre-determined coeffs]]*IF(SUM(biomassComponents26127[pre-determined coeffs])&gt;1,1/SUM(biomassComponents26127[pre-determined coeffs]),1)*(1-SUM(_xlfn._xlws.FILTER(biomassComponents26127[original coeffs from input],biomassComponents26127[pre-determined coeffs]=""))),biomassComponents26127[[#This Row],[original coeffs from input]])</f>
-        <v>8.5362609930616125E-3</v>
+        <v>8.5261972295296931E-3</v>
       </c>
       <c r="U10" s="75" t="str" cm="1">
         <f t="array" ref="U10">_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER(ROUND(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]*(biomassComponents26127[[#This Row],[normalized coeffs]]/biomassComponents26127[[#This Row],[original coeffs from input]])/(1000*biomassComponents26127[[#This Row],[normalized coeffs]]),6)&amp;" BIO-"&amp;mets27138[name],mets27138[category]=_xlfn.TEXTAFTER(O10,"BIOSYN-"),""))&amp;" --&gt; "&amp;biomassComponents26127[[#This Row],[product name]]</f>
@@ -16137,7 +16175,7 @@
       </c>
       <c r="V10" s="75" t="str" cm="1">
         <f t="array" ref="V10">_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER((-mets27138[normalized coeffs]*biomassComponents26127[[#This Row],[normalized coeffs]]/biomassComponents26127[[#This Row],[original coeffs from input]])&amp;" BIO-"&amp;mets27138[name],mets27138[category]=_xlfn.TEXTAFTER(P10,"BIOSYN-"),""))</f>
-        <v>0.000433013192175925 BIO-ca2_c + 3.83853063048642E-05 BIO-cu2_c + 0.000223577573565174 BIO-fe2_c + 0.20325693114852 BIO-k_c + 0.0214173173520482 BIO-mg2_c + 0.000031651042040853 BIO-mn2_c + 0.000530660024004088 BIO-zn2_c</v>
+        <v>0.000432502694385873 BIO-ca2_c + 3.83400522239421E-05 BIO-cu2_c + 0.000223313988392084 BIO-fe2_c + 0.203017302850725 BIO-k_c + 0.0213920675597218 BIO-mg2_c + 3.16137272723733E-05 BIO-mn2_c + 0.000530034406183621 BIO-zn2_c</v>
       </c>
       <c r="X10" s="78"/>
       <c r="Y10" t="s">
@@ -16187,11 +16225,11 @@
       </c>
       <c r="I11" s="72">
         <f>H11/($H$3)</f>
-        <v>-0.20076255966513035</v>
+        <v>-0.20052587208866396</v>
       </c>
       <c r="J11" s="37" cm="1">
         <f t="array" ref="J11">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-0.20076255966513035</v>
+        <v>-0.20052587208866396</v>
       </c>
       <c r="K11" t="str" cm="1">
         <f t="array" ref="K11">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -16203,7 +16241,7 @@
       </c>
       <c r="M11" s="73" cm="1">
         <f t="array" ref="M11">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-0.20076255966513035</v>
+        <v>-0.20052587208866396</v>
       </c>
       <c r="N11" s="73"/>
       <c r="O11" s="74" t="str">
@@ -16219,12 +16257,12 @@
       </c>
       <c r="R11" s="76" cm="1">
         <f t="array" ref="R11">SUM(_xlfn._xlws.FILTER(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]/1000,mets27138[category]=_xlfn.TEXTAFTER(O11,"BIOSYN-"),""))</f>
-        <v>0.14962526854278405</v>
+        <v>0.14944886890806833</v>
       </c>
       <c r="S11" s="76"/>
       <c r="T11" s="76" cm="1">
         <f t="array" ref="T11">IF(biomassComponents26127[[#This Row],[pre-determined coeffs]]&lt;&gt;"",biomassComponents26127[[#This Row],[pre-determined coeffs]]*IF(SUM(biomassComponents26127[pre-determined coeffs])&gt;1,1/SUM(biomassComponents26127[pre-determined coeffs]),1)*(1-SUM(_xlfn._xlws.FILTER(biomassComponents26127[original coeffs from input],biomassComponents26127[pre-determined coeffs]=""))),biomassComponents26127[[#This Row],[original coeffs from input]])</f>
-        <v>0.14962526854278405</v>
+        <v>0.14944886890806833</v>
       </c>
       <c r="U11" s="75" t="str" cm="1">
         <f t="array" ref="U11">_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER(ROUND(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]*(biomassComponents26127[[#This Row],[normalized coeffs]]/biomassComponents26127[[#This Row],[original coeffs from input]])/(1000*biomassComponents26127[[#This Row],[normalized coeffs]]),6)&amp;" BIO-"&amp;mets27138[name],mets27138[category]=_xlfn.TEXTAFTER(O11,"BIOSYN-"),""))&amp;" --&gt; "&amp;biomassComponents26127[[#This Row],[product name]]</f>
@@ -16232,7 +16270,7 @@
       </c>
       <c r="V11" s="75" t="str" cm="1">
         <f t="array" ref="V11">_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER((-mets27138[normalized coeffs]*biomassComponents26127[[#This Row],[normalized coeffs]]/biomassComponents26127[[#This Row],[original coeffs from input]])&amp;" BIO-"&amp;mets27138[name],mets27138[category]=_xlfn.TEXTAFTER(P11,"BIOSYN-"),""))</f>
-        <v>0.00228224215907342 BIO-ergstest_c</v>
+        <v>0.00227955152608666 BIO-ergstest_c</v>
       </c>
       <c r="X11" s="79" t="s">
         <v>54</v>
@@ -16284,11 +16322,11 @@
       </c>
       <c r="I12" s="72">
         <f>H12/($H$3)</f>
-        <v>-5.2832323430447602E-2</v>
+        <v>-5.2770037142542629E-2</v>
       </c>
       <c r="J12" s="37" cm="1">
         <f t="array" ref="J12">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-5.2832323430447602E-2</v>
+        <v>-5.2770037142542629E-2</v>
       </c>
       <c r="K12" t="str" cm="1">
         <f t="array" ref="K12">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -16300,7 +16338,7 @@
       </c>
       <c r="M12" s="73" cm="1">
         <f t="array" ref="M12">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-5.2832323430447602E-2</v>
+        <v>-5.2770037142542629E-2</v>
       </c>
       <c r="N12" s="73"/>
       <c r="O12" s="74" t="str">
@@ -16315,19 +16353,19 @@
       </c>
       <c r="R12" s="76" cm="1">
         <f t="array" ref="R12">SUM(_xlfn._xlws.FILTER(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]/1000,mets27138[category]=_xlfn.TEXTAFTER(O12,"BIOSYN-"),""))</f>
-        <v>3.4145053399876725E-3</v>
+        <v>3.410479833463442E-3</v>
       </c>
       <c r="S12" s="85">
         <v>58.068009171159375</v>
       </c>
       <c r="T12" s="76" cm="1">
         <f t="array" ref="T12">IF(biomassComponents26127[[#This Row],[pre-determined coeffs]]&lt;&gt;"",biomassComponents26127[[#This Row],[pre-determined coeffs]]*IF(SUM(biomassComponents26127[pre-determined coeffs])&gt;1,1/SUM(biomassComponents26127[pre-determined coeffs]),1)*(1-SUM(_xlfn._xlws.FILTER(biomassComponents26127[original coeffs from input],biomassComponents26127[pre-determined coeffs]=""))),biomassComponents26127[[#This Row],[original coeffs from input]])</f>
-        <v>0.11458616090831396</v>
+        <v>0.1151356589973577</v>
       </c>
       <c r="U12" s="75"/>
       <c r="V12" s="75" t="str" cm="1">
         <f t="array" ref="V12">_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER((-mets27138[normalized coeffs]*biomassComponents26127[[#This Row],[normalized coeffs]]/biomassComponents26127[[#This Row],[original coeffs from input]])&amp;" BIO-"&amp;mets27138[name],mets27138[category]=_xlfn.TEXTAFTER(P12,"BIOSYN-"),""))</f>
-        <v>1.19386325712368 BIO-pi_c</v>
+        <v>1.19958842998198 BIO-pi_c</v>
       </c>
       <c r="X12" s="79" t="s">
         <v>54</v>
@@ -16377,11 +16415,11 @@
       </c>
       <c r="I13" s="72">
         <f>H13/($H$3)</f>
-        <v>-4.7466461664883424E-3</v>
+        <v>-4.7410501421132623E-3</v>
       </c>
       <c r="J13" s="37" cm="1">
         <f t="array" ref="J13">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-4.7466461664883424E-3</v>
+        <v>-4.7410501421132623E-3</v>
       </c>
       <c r="K13" t="str" cm="1">
         <f t="array" ref="K13">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -16393,7 +16431,7 @@
       </c>
       <c r="M13" s="73" cm="1">
         <f t="array" ref="M13">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-4.7466461664883424E-3</v>
+        <v>-4.7410501421132623E-3</v>
       </c>
       <c r="N13" s="73"/>
       <c r="O13" s="74" t="str">
@@ -16409,21 +16447,21 @@
       </c>
       <c r="R13" s="76" cm="1">
         <f t="array" ref="R13">SUM(_xlfn._xlws.FILTER(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]/1000,mets27138[category]=_xlfn.TEXTAFTER(O13,"BIOSYN-"),""))</f>
-        <v>0.17386875801191395</v>
+        <v>0.17366377668957125</v>
       </c>
       <c r="S13" s="83">
         <v>8.5726740954505853</v>
       </c>
       <c r="T13" s="76" cm="1">
         <f t="array" ref="T13">IF(biomassComponents26127[[#This Row],[pre-determined coeffs]]&lt;&gt;"",biomassComponents26127[[#This Row],[pre-determined coeffs]]*IF(SUM(biomassComponents26127[pre-determined coeffs])&gt;1,1/SUM(biomassComponents26127[pre-determined coeffs]),1)*(1-SUM(_xlfn._xlws.FILTER(biomassComponents26127[original coeffs from input],biomassComponents26127[pre-determined coeffs]=""))),biomassComponents26127[[#This Row],[original coeffs from input]])</f>
-        <v>1.6916540231651671E-2</v>
+        <v>1.6997663523128047E-2</v>
       </c>
       <c r="U13" s="80" t="s">
         <v>89</v>
       </c>
       <c r="V13" s="75" t="str" cm="1">
         <f t="array" ref="V13">_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER((-mets27138[normalized coeffs]*biomassComponents26127[[#This Row],[normalized coeffs]]/biomassComponents26127[[#This Row],[original coeffs from input]])&amp;" BIO-"&amp;mets27138[name],mets27138[category]=_xlfn.TEXTAFTER(P13,"BIOSYN-"),""))</f>
-        <v>0.0150867216271455 BIO-alatrna_c + 0.00596057135849649 BIO-argtrna_c + 0.00716504288031904 BIO-asntrna_c + 0.00716504288031904 BIO-asptrna_c + 0.000216186356212452 BIO-cystrna_c + 0.0119520030818289 BIO-glntrna_c + 0.0119520030818289 BIO-glutrna_c + 0.0137278172392546 BIO-glytrna_c + 0.00298028567924824 BIO-histrna_c + 0.00909525714334093 BIO-iletrna_c + 0.0123689456118358 BIO-leutrna_c + 0.0101453285595673 BIO-lystrna_c + 0.00176038397500774 BIO-mettrna_c + 0.00580613849242807 BIO-phetrna_c + 0.00651648381168168 BIO-protrna_c + 0.00823051171849112 BIO-sertrna_c + 0.00860113094077199 BIO-thrtrna_c + 0.00100371534802805 BIO-trptrna_c + 0.00302660898697433 BIO-tyrtrna_c + 0.0113189069560817 BIO-valtrna_c</v>
+        <v>0.0151590700210383 BIO-alatrna_c + 0.00598915528647819 BIO-argtrna_c + 0.0071994028531067 BIO-asntrna_c + 0.0071994028531067 BIO-asptrna_c + 0.000217223078174986 BIO-cystrna_c + 0.0120093189287134 BIO-glntrna_c + 0.0120093189287134 BIO-glutrna_c + 0.013793649005324 BIO-glytrna_c + 0.00299457764323909 BIO-histrna_c + 0.00913887346122792 BIO-iletrna_c + 0.0124282609071849 BIO-leutrna_c + 0.0101939804963458 BIO-lystrna_c + 0.00176882589873206 BIO-mettrna_c + 0.00583398183739244 BIO-phetrna_c + 0.00654773361858174 BIO-protrna_c + 0.00826998114852798 BIO-sertrna_c + 0.00864237767578872 BIO-thrtrna_c + 0.00100852866633205 BIO-trptrna_c + 0.0030411230944498 BIO-tyrtrna_c + 0.0113731867896421 BIO-valtrna_c</v>
       </c>
       <c r="X13" s="79" t="s">
         <v>54</v>
@@ -16469,11 +16507,11 @@
       </c>
       <c r="I14" s="72">
         <f>H14/($H$3)</f>
-        <v>-9.6790570126994366E-2</v>
+        <v>-9.6676459580155499E-2</v>
       </c>
       <c r="J14" s="37" cm="1">
         <f t="array" ref="J14">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-9.6790570126994366E-2</v>
+        <v>-9.6676459580155499E-2</v>
       </c>
       <c r="K14" t="str" cm="1">
         <f t="array" ref="K14">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -16485,7 +16523,7 @@
       </c>
       <c r="M14" s="73" cm="1">
         <f t="array" ref="M14">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-9.6790570126994366E-2</v>
+        <v>-9.6676459580155499E-2</v>
       </c>
       <c r="N14" s="73"/>
       <c r="O14" s="74" t="str">
@@ -16501,20 +16539,20 @@
       </c>
       <c r="R14" s="76" cm="1">
         <f t="array" ref="R14">SUM(_xlfn._xlws.FILTER(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]/1000,mets27138[category]=_xlfn.TEXTAFTER(O14,"BIOSYN-"),""))</f>
-        <v>0.56409360646284412</v>
+        <v>0.56342857236068589</v>
       </c>
       <c r="S14" s="83"/>
       <c r="T14" s="76" cm="1">
         <f t="array" ref="T14">IF(biomassComponents26127[[#This Row],[pre-determined coeffs]]&lt;&gt;"",biomassComponents26127[[#This Row],[pre-determined coeffs]]*IF(SUM(biomassComponents26127[pre-determined coeffs])&gt;1,1/SUM(biomassComponents26127[pre-determined coeffs]),1)*(1-SUM(_xlfn._xlws.FILTER(biomassComponents26127[original coeffs from input],biomassComponents26127[pre-determined coeffs]=""))),biomassComponents26127[[#This Row],[original coeffs from input]])</f>
-        <v>0.56409360646284412</v>
+        <v>0.56342857236068589</v>
       </c>
       <c r="U14" s="75" t="str" cm="1">
         <f t="array" ref="U14">_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER(ROUND(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]*(biomassComponents26127[[#This Row],[original coeffs from input]])/(1000*biomassComponents26127[[#This Row],[normalized coeffs]]),6)&amp;" BIO-"&amp;mets27138[name],mets27138[category]=_xlfn.TEXTAFTER(O14,"BIOSYN-"),""))&amp;" --&gt; "&amp;biomassComponents26127[[#This Row],[product name]]</f>
-        <v>0.009601 BIO-ctp_c + 0.01118 BIO-gtp_c + 0.012907 BIO-utp_c + 0.530405 BIO-atp_c --&gt; BIO-rna</v>
+        <v>0.00959 BIO-ctp_c + 0.011167 BIO-gtp_c + 0.012892 BIO-utp_c + 0.52978 BIO-atp_c --&gt; BIO-rna</v>
       </c>
       <c r="V14" s="75" t="str" cm="1">
         <f t="array" ref="V14">_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER((-mets27138[normalized coeffs]*biomassComponents26127[[#This Row],[normalized coeffs]]/biomassComponents26127[[#This Row],[original coeffs from input]])&amp;" BIO-"&amp;mets27138[name],mets27138[category]=_xlfn.TEXTAFTER(P14,"BIOSYN-"),""))</f>
-        <v>0.0315641700318472 BIO-ctp_c + 0.0324823869642452 BIO-gtp_c + 0.0422975771290416 BIO-utp_c + 1.61611230800235 BIO-atp_c</v>
+        <v>0.0315269576804981 BIO-ctp_c + 0.0324440920876445 BIO-gtp_c + 0.042247710704556 BIO-utp_c + 1.61420700401481 BIO-atp_c</v>
       </c>
       <c r="X14" s="79" t="s">
         <v>54</v>
@@ -16560,11 +16598,11 @@
       </c>
       <c r="I15" s="72">
         <f>H15/($H$3)</f>
-        <v>-4.8517006890069179E-3</v>
+        <v>-4.8459808113577351E-3</v>
       </c>
       <c r="J15" s="37" cm="1">
         <f t="array" ref="J15">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-4.8517006890069179E-3</v>
+        <v>-4.8459808113577351E-3</v>
       </c>
       <c r="K15" t="str" cm="1">
         <f t="array" ref="K15">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -16576,7 +16614,7 @@
       </c>
       <c r="M15" s="73" cm="1">
         <f t="array" ref="M15">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-4.8517006890069179E-3</v>
+        <v>-4.8459808113577351E-3</v>
       </c>
       <c r="N15" s="73"/>
       <c r="O15" s="73" t="str">
@@ -16595,7 +16633,7 @@
       </c>
       <c r="Z15" s="77" t="str" cm="1">
         <f t="array" ref="Z15">_xlfn.LET(_xlpm.RNAmass,_xlfn.XLOOKUP("BIOSYN-RNA",biomassComponents26127[rxn name],biomassComponents26127[normalized coeffs],0),_xlpm.coeff,1/_xlpm.RNAmass,_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER(ROUND(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]/(1000),6)*_xlpm.coeff&amp;" BIO-"&amp;mets27138[name],mets27138[category]="RNA",""))&amp;" --&gt; "&amp;SUBSTITUTE(LOWER(ExtraRxns25116[[#This Row],[name]]),"biosyn-","BIO-"))</f>
-        <v>0.0170202248173015 BIO-ctp_c + 0.0198194056303959 BIO-gtp_c + 0.0228809542461109 BIO-utp_c + 0.940278340195896 BIO-atp_c --&gt; BIO-trna</v>
+        <v>0.0170207910468922 BIO-ctp_c + 0.0198197261335396 BIO-gtp_c + 0.0228813387045395 BIO-utp_c + 0.940278903109753 BIO-atp_c --&gt; BIO-trna</v>
       </c>
     </row>
     <row r="16" spans="1:33" ht="16" x14ac:dyDescent="0.2">
@@ -16632,11 +16670,11 @@
       </c>
       <c r="I16" s="72">
         <f>H16/($H$3)</f>
-        <v>-1.3310273317818271E-3</v>
+        <v>-1.3294581266775714E-3</v>
       </c>
       <c r="J16" s="37" cm="1">
         <f t="array" ref="J16">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-1.3310273317818271E-3</v>
+        <v>-1.3294581266775714E-3</v>
       </c>
       <c r="K16" t="str" cm="1">
         <f t="array" ref="K16">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -16648,11 +16686,14 @@
       </c>
       <c r="M16" s="73" cm="1">
         <f t="array" ref="M16">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-4.8861097621396361E-4</v>
+        <v>-4.909541108088141E-4</v>
       </c>
       <c r="N16" s="73"/>
       <c r="O16" s="73"/>
-      <c r="P16" s="60"/>
+      <c r="P16" s="60" cm="1">
+        <f t="array" ref="P16:P19">E16:E19*F16:F19/1000</f>
+        <v>-1.2341210697529999E-3</v>
+      </c>
       <c r="Q16" s="81"/>
       <c r="R16" s="29"/>
       <c r="S16" s="73"/>
@@ -16665,7 +16706,7 @@
       </c>
       <c r="Z16" s="77" t="str" cm="1">
         <f t="array" ref="Z16">_xlfn.LET(_xlpm.RNAmass,_xlfn.XLOOKUP("BIOSYN-RNA",biomassComponents26127[rxn name],biomassComponents26127[normalized coeffs],0),_xlpm.coeff,1/_xlpm.RNAmass,_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER(ROUND(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]/(1000),6)*_xlpm.coeff&amp;" BIO-"&amp;mets27138[name],mets27138[category]="RNA",""))&amp;" --&gt; "&amp;SUBSTITUTE(LOWER(ExtraRxns25116[[#This Row],[name]]),"biosyn-","BIO-"))</f>
-        <v>0.0170202248173015 BIO-ctp_c + 0.0198194056303959 BIO-gtp_c + 0.0228809542461109 BIO-utp_c + 0.940278340195896 BIO-atp_c --&gt; BIO-rrna</v>
+        <v>0.0170207910468922 BIO-ctp_c + 0.0198197261335396 BIO-gtp_c + 0.0228813387045395 BIO-utp_c + 0.940278903109753 BIO-atp_c --&gt; BIO-rrna</v>
       </c>
     </row>
     <row r="17" spans="1:26" ht="16" x14ac:dyDescent="0.2">
@@ -16702,11 +16743,11 @@
       </c>
       <c r="I17" s="72">
         <f>H17/($H$3)</f>
-        <v>-8.9835085281910311E-4</v>
+        <v>-8.9729174853927661E-4</v>
       </c>
       <c r="J17" s="37" cm="1">
         <f t="array" ref="J17">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-8.9835085281910311E-4</v>
+        <v>-8.9729174853927661E-4</v>
       </c>
       <c r="K17" t="str" cm="1">
         <f t="array" ref="K17">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -16718,11 +16759,13 @@
       </c>
       <c r="M17" s="73" cm="1">
         <f t="array" ref="M17">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-3.2977841754081835E-4</v>
+        <v>-3.313598703865206E-4</v>
       </c>
       <c r="N17" s="73"/>
       <c r="O17" s="73"/>
-      <c r="P17" s="73"/>
+      <c r="P17" s="73">
+        <v>-7.6884796786799996E-4</v>
+      </c>
       <c r="Q17" s="82"/>
       <c r="R17" s="73"/>
       <c r="S17" s="73"/>
@@ -16735,7 +16778,7 @@
       </c>
       <c r="Z17" s="77" t="str" cm="1">
         <f t="array" ref="Z17">_xlfn.LET(_xlpm.RNAmass,_xlfn.XLOOKUP("BIOSYN-RNA",biomassComponents26127[rxn name],biomassComponents26127[normalized coeffs],0),_xlpm.coeff,1/_xlpm.RNAmass,_xlfn.TEXTJOIN(" + ",TRUE,_xlfn._xlws.FILTER(ROUND(-mets27138[MW for biomass normalization (g/mol)]*mets27138[normalized coeffs]/(1000),6)*_xlpm.coeff&amp;" BIO-"&amp;mets27138[name],mets27138[category]="RNA",""))&amp;" --&gt; "&amp;SUBSTITUTE(LOWER(ExtraRxns25116[[#This Row],[name]]),"biosyn-","BIO-"))</f>
-        <v>0.0170202248173015 BIO-ctp_c + 0.0198194056303959 BIO-gtp_c + 0.0228809542461109 BIO-utp_c + 0.940278340195896 BIO-atp_c --&gt; BIO-mrna</v>
+        <v>0.0170207910468922 BIO-ctp_c + 0.0198197261335396 BIO-gtp_c + 0.0228813387045395 BIO-utp_c + 0.940278903109753 BIO-atp_c --&gt; BIO-mrna</v>
       </c>
     </row>
     <row r="18" spans="1:26" ht="16" x14ac:dyDescent="0.2">
@@ -16772,11 +16815,11 @@
       </c>
       <c r="I18" s="72">
         <f>H18/($H$3)</f>
-        <v>-8.9835085281910311E-4</v>
+        <v>-8.9729174853927661E-4</v>
       </c>
       <c r="J18" s="37" cm="1">
         <f t="array" ref="J18">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-8.9835085281910311E-4</v>
+        <v>-8.9729174853927661E-4</v>
       </c>
       <c r="K18" t="str" cm="1">
         <f t="array" ref="K18">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -16788,11 +16831,13 @@
       </c>
       <c r="M18" s="73" cm="1">
         <f t="array" ref="M18">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-3.2977841754081835E-4</v>
+        <v>-3.313598703865206E-4</v>
       </c>
       <c r="N18" s="73"/>
       <c r="O18" s="73"/>
-      <c r="P18" s="73"/>
+      <c r="P18" s="73">
+        <v>-8.7563226666799985E-4</v>
+      </c>
       <c r="Q18" s="73"/>
       <c r="R18" s="82"/>
       <c r="S18" s="73"/>
@@ -16834,11 +16879,11 @@
       </c>
       <c r="I19" s="72">
         <f>H19/($H$3)</f>
-        <v>-1.3310273317818271E-3</v>
+        <v>-1.3294581266775714E-3</v>
       </c>
       <c r="J19" s="37" cm="1">
         <f t="array" ref="J19">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-1.3310273317818271E-3</v>
+        <v>-1.3294581266775714E-3</v>
       </c>
       <c r="K19" t="str" cm="1">
         <f t="array" ref="K19">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -16850,11 +16895,13 @@
       </c>
       <c r="M19" s="73" cm="1">
         <f t="array" ref="M19">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-4.8861097621396361E-4</v>
+        <v>-4.909541108088141E-4</v>
       </c>
       <c r="N19" s="73"/>
       <c r="O19" s="73"/>
-      <c r="P19" s="73"/>
+      <c r="P19" s="73">
+        <v>-1.198491257673E-3</v>
+      </c>
       <c r="Q19" s="73"/>
       <c r="R19" s="73"/>
       <c r="S19" s="73"/>
@@ -16896,11 +16943,11 @@
       </c>
       <c r="I20" s="72">
         <f>H20/($H$3)</f>
-        <v>1.5836299210381055</v>
+        <v>1.5817629119271668</v>
       </c>
       <c r="J20" s="37" cm="1">
         <f t="array" ref="J20">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-127.13931207896188</v>
+        <v>-127.14117908807282</v>
       </c>
       <c r="K20" t="str" cm="1">
         <f t="array" ref="K20">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -16912,7 +16959,7 @@
       </c>
       <c r="M20" s="73" cm="1">
         <f t="array" ref="M20">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-137.8793120789619</v>
+        <v>-137.88117908807283</v>
       </c>
       <c r="N20" s="73"/>
       <c r="O20" s="73"/>
@@ -16978,7 +17025,9 @@
       </c>
       <c r="N21" s="73"/>
       <c r="O21" s="73"/>
-      <c r="P21" s="73"/>
+      <c r="P21" s="73" t="s">
+        <v>585</v>
+      </c>
       <c r="Q21" s="73"/>
       <c r="R21" s="73"/>
       <c r="S21" s="73"/>
@@ -17040,7 +17089,10 @@
       </c>
       <c r="N22" s="73"/>
       <c r="O22" s="73"/>
-      <c r="P22" s="73"/>
+      <c r="P22" s="73" cm="1">
+        <f t="array" ref="P22:P27">E10:E15*F10:F15/1000</f>
+        <v>-6.2299282737999999E-2</v>
+      </c>
       <c r="Q22" s="73"/>
       <c r="R22" s="73"/>
       <c r="S22" s="73"/>
@@ -17082,11 +17134,11 @@
       </c>
       <c r="I23" s="72">
         <f>H23/($H$3)</f>
-        <v>-8.9144823194849156E-3</v>
+        <v>-8.9039726546391862E-3</v>
       </c>
       <c r="J23" s="37" cm="1">
         <f t="array" ref="J23">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-8.9144823194849156E-3</v>
+        <v>-8.9039726546391862E-3</v>
       </c>
       <c r="K23" t="str" cm="1">
         <f t="array" ref="K23">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -17098,11 +17150,13 @@
       </c>
       <c r="M23" s="73" cm="1">
         <f t="array" ref="M23">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-2.0887043481275201E-3</v>
+        <v>-1.9672719034771252E-3</v>
       </c>
       <c r="N23" s="73"/>
       <c r="O23" s="73"/>
-      <c r="P23" s="73"/>
+      <c r="P23" s="73">
+        <v>-9.6675035625200009E-2</v>
+      </c>
       <c r="Q23" s="73"/>
       <c r="R23" s="73"/>
       <c r="S23" s="73"/>
@@ -17144,11 +17198,11 @@
       </c>
       <c r="I24" s="72">
         <f>H24/($H$3)</f>
-        <v>-2.3172603332462776E-3</v>
+        <v>-2.3145284158348207E-3</v>
       </c>
       <c r="J24" s="37" cm="1">
         <f t="array" ref="J24">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-2.3172603332462776E-3</v>
+        <v>-2.3145284158348207E-3</v>
       </c>
       <c r="K24" t="str" cm="1">
         <f t="array" ref="K24">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -17160,11 +17214,13 @@
       </c>
       <c r="M24" s="73" cm="1">
         <f t="array" ref="M24">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-5.4294479032345974E-4</v>
+        <v>-5.1137923473954959E-4</v>
       </c>
       <c r="N24" s="73"/>
       <c r="O24" s="73"/>
-      <c r="P24" s="73"/>
+      <c r="P24" s="73">
+        <v>-2.54408329836E-2</v>
+      </c>
       <c r="Q24" s="73"/>
       <c r="R24" s="73"/>
       <c r="S24" s="73"/>
@@ -17206,11 +17262,11 @@
       </c>
       <c r="I25" s="72">
         <f>H25/($H$3)</f>
-        <v>-8.6461218885640675E-3</v>
+        <v>-8.6359286053191708E-3</v>
       </c>
       <c r="J25" s="37" cm="1">
         <f t="array" ref="J25">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-8.6461218885640675E-3</v>
+        <v>-8.6359286053191708E-3</v>
       </c>
       <c r="K25" t="str" cm="1">
         <f t="array" ref="K25">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -17222,11 +17278,13 @@
       </c>
       <c r="M25" s="73" cm="1">
         <f t="array" ref="M25">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-2.0258262606692528E-3</v>
+        <v>-1.9080494027378895E-3</v>
       </c>
       <c r="N25" s="73"/>
       <c r="O25" s="73"/>
-      <c r="P25" s="73"/>
+      <c r="P25" s="73">
+        <v>-2.8644049544399998E-3</v>
+      </c>
       <c r="Q25" s="73"/>
       <c r="R25" s="73"/>
       <c r="S25" s="73"/>
@@ -17268,11 +17326,11 @@
       </c>
       <c r="I26" s="72">
         <f>H26/($H$3)</f>
-        <v>-2.3236578842970881E-3</v>
+        <v>-2.3209184245388112E-3</v>
       </c>
       <c r="J26" s="37" cm="1">
         <f t="array" ref="J26">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-2.3236578842970881E-3</v>
+        <v>-2.3209184245388112E-3</v>
       </c>
       <c r="K26" t="str" cm="1">
         <f t="array" ref="K26">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -17284,11 +17342,13 @@
       </c>
       <c r="M26" s="73" cm="1">
         <f t="array" ref="M26">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-5.4444376605960402E-4</v>
+        <v>-5.1279106348992032E-4</v>
       </c>
       <c r="N26" s="73"/>
       <c r="O26" s="73"/>
-      <c r="P26" s="73"/>
+      <c r="P26" s="73">
+        <v>-4.6608450454200007E-2</v>
+      </c>
       <c r="Q26" s="73"/>
       <c r="R26" s="73"/>
       <c r="S26" s="73"/>
@@ -17330,11 +17390,11 @@
       </c>
       <c r="I27" s="72">
         <f>H27/($H$3)</f>
-        <v>-1.9956992146397392E-3</v>
+        <v>-1.993346399397411E-3</v>
       </c>
       <c r="J27" s="37" cm="1">
         <f t="array" ref="J27">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-1.9956992146397392E-3</v>
+        <v>-1.993346399397411E-3</v>
       </c>
       <c r="K27" t="str" cm="1">
         <f t="array" ref="K27">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -17346,11 +17406,13 @@
       </c>
       <c r="M27" s="73" cm="1">
         <f t="array" ref="M27">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-4.6760153621725446E-4</v>
+        <v>-4.4041626333933597E-4</v>
       </c>
       <c r="N27" s="73"/>
       <c r="O27" s="73"/>
-      <c r="P27" s="73"/>
+      <c r="P27" s="73">
+        <v>-4.932149980319999E-3</v>
+      </c>
       <c r="Q27" s="73"/>
       <c r="R27" s="73"/>
       <c r="S27" s="73"/>
@@ -17392,11 +17454,11 @@
       </c>
       <c r="I28" s="72">
         <f>H28/($H$3)</f>
-        <v>-2.2994145329466474E-3</v>
+        <v>-2.2967036547131637E-3</v>
       </c>
       <c r="J28" s="37" cm="1">
         <f t="array" ref="J28">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-2.2994145329466474E-3</v>
+        <v>-2.2967036547131637E-3</v>
       </c>
       <c r="K28" t="str" cm="1">
         <f t="array" ref="K28">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -17408,7 +17470,7 @@
       </c>
       <c r="M28" s="73" cm="1">
         <f t="array" ref="M28">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-5.3876343695421472E-4</v>
+        <v>-5.0744097559377857E-4</v>
       </c>
       <c r="N28" s="73"/>
       <c r="O28" s="73"/>
@@ -17454,11 +17516,11 @@
       </c>
       <c r="I29" s="72">
         <f>H29/($H$3)</f>
-        <v>-4.3301319217592458E-4</v>
+        <v>-4.3250269438587326E-4</v>
       </c>
       <c r="J29" s="37" cm="1">
         <f t="array" ref="J29">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-4.3301319217592458E-4</v>
+        <v>-4.3250269438587326E-4</v>
       </c>
       <c r="K29" t="str" cm="1">
         <f t="array" ref="K29">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -17470,7 +17532,7 @@
       </c>
       <c r="M29" s="73" cm="1">
         <f t="array" ref="M29">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-4.3301319217592458E-4</v>
+        <v>-4.3250269438587326E-4</v>
       </c>
       <c r="N29" s="73"/>
       <c r="O29" s="73"/>
@@ -17516,11 +17578,11 @@
       </c>
       <c r="I30" s="72">
         <f>H30/($H$3)</f>
-        <v>-3.838530630486423E-5</v>
+        <v>-3.8340052223942106E-5</v>
       </c>
       <c r="J30" s="37" cm="1">
         <f t="array" ref="J30">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-3.838530630486423E-5</v>
+        <v>-3.8340052223942106E-5</v>
       </c>
       <c r="K30" t="str" cm="1">
         <f t="array" ref="K30">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -17532,7 +17594,7 @@
       </c>
       <c r="M30" s="73" cm="1">
         <f t="array" ref="M30">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-3.838530630486423E-5</v>
+        <v>-3.8340052223942106E-5</v>
       </c>
       <c r="N30" s="73"/>
       <c r="O30" s="73"/>
@@ -17578,11 +17640,11 @@
       </c>
       <c r="I31" s="72">
         <f>H31/($H$3)</f>
-        <v>-2.2357757356517409E-4</v>
+        <v>-2.2331398839208383E-4</v>
       </c>
       <c r="J31" s="37" cm="1">
         <f t="array" ref="J31">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-2.2357757356517409E-4</v>
+        <v>-2.2331398839208383E-4</v>
       </c>
       <c r="K31" t="str" cm="1">
         <f t="array" ref="K31">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -17594,7 +17656,7 @@
       </c>
       <c r="M31" s="73" cm="1">
         <f t="array" ref="M31">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-2.2357757356517409E-4</v>
+        <v>-2.2331398839208383E-4</v>
       </c>
       <c r="N31" s="73"/>
       <c r="O31" s="73"/>
@@ -17640,11 +17702,11 @@
       </c>
       <c r="I32" s="72">
         <f>H32/($H$3)</f>
-        <v>-0.20325693114852011</v>
+        <v>-0.20301730285072503</v>
       </c>
       <c r="J32" s="37" cm="1">
         <f t="array" ref="J32">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-0.20325693114852011</v>
+        <v>-0.20301730285072503</v>
       </c>
       <c r="K32" t="str" cm="1">
         <f t="array" ref="K32">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -17656,7 +17718,7 @@
       </c>
       <c r="M32" s="73" cm="1">
         <f t="array" ref="M32">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-0.20325693114852011</v>
+        <v>-0.20301730285072503</v>
       </c>
       <c r="N32" s="73"/>
       <c r="O32" s="73"/>
@@ -17702,11 +17764,11 @@
       </c>
       <c r="I33" s="72">
         <f>H33/($H$3)</f>
-        <v>-2.1417317352048236E-2</v>
+        <v>-2.1392067559721801E-2</v>
       </c>
       <c r="J33" s="37" cm="1">
         <f t="array" ref="J33">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-2.1417317352048236E-2</v>
+        <v>-2.1392067559721801E-2</v>
       </c>
       <c r="K33" t="str" cm="1">
         <f t="array" ref="K33">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -17718,7 +17780,7 @@
       </c>
       <c r="M33" s="73" cm="1">
         <f t="array" ref="M33">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-2.1417317352048236E-2</v>
+        <v>-2.1392067559721801E-2</v>
       </c>
       <c r="N33" s="73"/>
       <c r="O33" s="73"/>
@@ -17764,11 +17826,11 @@
       </c>
       <c r="I34" s="72">
         <f>H34/($H$3)</f>
-        <v>-3.1651042040852962E-5</v>
+        <v>-3.1613727272373316E-5</v>
       </c>
       <c r="J34" s="37" cm="1">
         <f t="array" ref="J34">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-3.1651042040852962E-5</v>
+        <v>-3.1613727272373316E-5</v>
       </c>
       <c r="K34" t="str" cm="1">
         <f t="array" ref="K34">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -17780,7 +17842,7 @@
       </c>
       <c r="M34" s="73" cm="1">
         <f t="array" ref="M34">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-3.1651042040852962E-5</v>
+        <v>-3.1613727272373316E-5</v>
       </c>
       <c r="N34" s="73"/>
       <c r="O34" s="73"/>
@@ -17826,11 +17888,11 @@
       </c>
       <c r="I35" s="72">
         <f>H35/($H$3)</f>
-        <v>-5.3066002400408796E-4</v>
+        <v>-5.3003440618362067E-4</v>
       </c>
       <c r="J35" s="37" cm="1">
         <f t="array" ref="J35">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-5.3066002400408796E-4</v>
+        <v>-5.3003440618362067E-4</v>
       </c>
       <c r="K35" t="str" cm="1">
         <f t="array" ref="K35">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -17842,7 +17904,7 @@
       </c>
       <c r="M35" s="73" cm="1">
         <f t="array" ref="M35">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-5.3066002400408796E-4</v>
+        <v>-5.3003440618362067E-4</v>
       </c>
       <c r="N35" s="73"/>
       <c r="O35" s="73"/>
@@ -17888,11 +17950,11 @@
       </c>
       <c r="I36" s="72">
         <f>H36/($H$3)</f>
-        <v>-2.2822421590734188E-3</v>
+        <v>-2.2795515260866633E-3</v>
       </c>
       <c r="J36" s="37" cm="1">
         <f t="array" ref="J36">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-2.2822421590734188E-3</v>
+        <v>-2.2795515260866633E-3</v>
       </c>
       <c r="K36" t="str" cm="1">
         <f t="array" ref="K36">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -17904,7 +17966,7 @@
       </c>
       <c r="M36" s="73" cm="1">
         <f t="array" ref="M36">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-2.2822421590734188E-3</v>
+        <v>-2.2795515260866633E-3</v>
       </c>
       <c r="N36" s="73"/>
       <c r="O36" s="73"/>
@@ -17950,11 +18012,11 @@
       </c>
       <c r="I37" s="72">
         <f>H37/($H$3)</f>
-        <v>-3.5575434540700314E-2</v>
+        <v>-3.553349313789482E-2</v>
       </c>
       <c r="J37" s="37" cm="1">
         <f t="array" ref="J37">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>128.68736656545929</v>
+        <v>128.68740850686208</v>
       </c>
       <c r="K37" t="str" cm="1">
         <f t="array" ref="K37">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -17966,7 +18028,7 @@
       </c>
       <c r="M37" s="73" cm="1">
         <f t="array" ref="M37">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>138.26907874287633</v>
+        <v>138.26335357001801</v>
       </c>
       <c r="N37" s="73"/>
       <c r="O37" s="73"/>
@@ -18012,11 +18074,11 @@
       </c>
       <c r="I38" s="72">
         <f>H38/($H$3)</f>
-        <v>-0.15506182209027067</v>
+        <v>-0.15487901306983265</v>
       </c>
       <c r="J38" s="37" cm="1">
         <f t="array" ref="J38">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-0.15506182209027067</v>
+        <v>-0.15487901306983265</v>
       </c>
       <c r="K38" t="str" cm="1">
         <f t="array" ref="K38">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -18028,7 +18090,7 @@
       </c>
       <c r="M38" s="73" cm="1">
         <f t="array" ref="M38">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-1.5086721627145545E-2</v>
+        <v>-1.5159070021038282E-2</v>
       </c>
       <c r="N38" s="73"/>
       <c r="O38" s="73"/>
@@ -18077,11 +18139,11 @@
       </c>
       <c r="I39" s="72">
         <f>H39/($H$3)</f>
-        <v>-6.126294886256331E-2</v>
+        <v>-6.1190723349411599E-2</v>
       </c>
       <c r="J39" s="37" cm="1">
         <f t="array" ref="J39">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-6.126294886256331E-2</v>
+        <v>-6.1190723349411599E-2</v>
       </c>
       <c r="K39" t="str" cm="1">
         <f t="array" ref="K39">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -18093,7 +18155,7 @@
       </c>
       <c r="M39" s="73" cm="1">
         <f t="array" ref="M39">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-5.9605713584964881E-3</v>
+        <v>-5.9891552864781887E-3</v>
       </c>
       <c r="N39" s="73"/>
       <c r="O39" s="73"/>
@@ -18141,11 +18203,11 @@
       </c>
       <c r="I40" s="72">
         <f>H40/($H$3)</f>
-        <v>-7.3642546859095215E-2</v>
+        <v>-7.3555726507880503E-2</v>
       </c>
       <c r="J40" s="37" cm="1">
         <f t="array" ref="J40">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-7.3642546859095215E-2</v>
+        <v>-7.3555726507880503E-2</v>
       </c>
       <c r="K40" t="str" cm="1">
         <f t="array" ref="K40">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -18157,7 +18219,7 @@
       </c>
       <c r="M40" s="73" cm="1">
         <f t="array" ref="M40">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-7.1650428803190364E-3</v>
+        <v>-7.1994028531066952E-3</v>
       </c>
       <c r="N40" s="73"/>
       <c r="O40" s="73"/>
@@ -18205,11 +18267,11 @@
       </c>
       <c r="I41" s="72">
         <f>H41/($H$3)</f>
-        <v>-7.3642546859095215E-2</v>
+        <v>-7.3555726507880503E-2</v>
       </c>
       <c r="J41" s="37" cm="1">
         <f t="array" ref="J41">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-7.3642546859095215E-2</v>
+        <v>-7.3555726507880503E-2</v>
       </c>
       <c r="K41" t="str" cm="1">
         <f t="array" ref="K41">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -18221,7 +18283,7 @@
       </c>
       <c r="M41" s="73" cm="1">
         <f t="array" ref="M41">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-7.1650428803190364E-3</v>
+        <v>-7.1994028531066952E-3</v>
       </c>
       <c r="N41" s="73"/>
       <c r="O41" s="73"/>
@@ -18269,11 +18331,11 @@
       </c>
       <c r="I42" s="72">
         <f>H42/($H$3)</f>
-        <v>-2.2219704939105177E-3</v>
+        <v>-2.2193509177701222E-3</v>
       </c>
       <c r="J42" s="37" cm="1">
         <f t="array" ref="J42">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-2.2219704939105177E-3</v>
+        <v>-2.2193509177701222E-3</v>
       </c>
       <c r="K42" t="str" cm="1">
         <f t="array" ref="K42">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -18285,7 +18347,7 @@
       </c>
       <c r="M42" s="73" cm="1">
         <f t="array" ref="M42">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-2.1618635621245175E-4</v>
+        <v>-2.172230781749855E-4</v>
       </c>
       <c r="N42" s="73"/>
       <c r="O42" s="73"/>
@@ -18333,11 +18395,11 @@
       </c>
       <c r="I43" s="72">
         <f>H43/($H$3)</f>
-        <v>-0.12284308157196154</v>
+        <v>-0.12269825660404209</v>
       </c>
       <c r="J43" s="37" cm="1">
         <f t="array" ref="J43">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-0.12284308157196154</v>
+        <v>-0.12269825660404209</v>
       </c>
       <c r="K43" t="str" cm="1">
         <f t="array" ref="K43">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -18349,7 +18411,7 @@
       </c>
       <c r="M43" s="73" cm="1">
         <f t="array" ref="M43">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-1.195200308182888E-2</v>
+        <v>-1.2009318928713436E-2</v>
       </c>
       <c r="N43" s="73"/>
       <c r="O43" s="73"/>
@@ -18397,11 +18459,11 @@
       </c>
       <c r="I44" s="72">
         <f>H44/($H$3)</f>
-        <v>-0.12284308157196154</v>
+        <v>-0.12269825660404209</v>
       </c>
       <c r="J44" s="37" cm="1">
         <f t="array" ref="J44">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-0.12284308157196154</v>
+        <v>-0.12269825660404209</v>
       </c>
       <c r="K44" t="str" cm="1">
         <f t="array" ref="K44">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -18413,7 +18475,7 @@
       </c>
       <c r="M44" s="73" cm="1">
         <f t="array" ref="M44">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-1.195200308182888E-2</v>
+        <v>-1.2009318928713436E-2</v>
       </c>
       <c r="N44" s="73"/>
       <c r="O44" s="73"/>
@@ -18461,11 +18523,11 @@
       </c>
       <c r="I45" s="72">
         <f>H45/($H$3)</f>
-        <v>-0.14109495800671129</v>
+        <v>-0.14092861512027899</v>
       </c>
       <c r="J45" s="37" cm="1">
         <f t="array" ref="J45">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-0.14109495800671129</v>
+        <v>-0.14092861512027899</v>
       </c>
       <c r="K45" t="str" cm="1">
         <f t="array" ref="K45">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -18477,7 +18539,7 @@
       </c>
       <c r="M45" s="73" cm="1">
         <f t="array" ref="M45">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-1.3727817239254576E-2</v>
+        <v>-1.3793649005324024E-2</v>
       </c>
       <c r="N45" s="73"/>
       <c r="O45" s="73"/>
@@ -18525,11 +18587,11 @@
       </c>
       <c r="I46" s="72">
         <f>H46/($H$3)</f>
-        <v>-3.0631474431281655E-2</v>
+        <v>-3.05953616747058E-2</v>
       </c>
       <c r="J46" s="37" cm="1">
         <f t="array" ref="J46">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-3.0631474431281655E-2</v>
+        <v>-3.05953616747058E-2</v>
       </c>
       <c r="K46" t="str" cm="1">
         <f t="array" ref="K46">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -18541,7 +18603,7 @@
       </c>
       <c r="M46" s="73" cm="1">
         <f t="array" ref="M46">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-2.9802856792482441E-3</v>
+        <v>-2.9945776432390944E-3</v>
       </c>
       <c r="N46" s="73"/>
       <c r="O46" s="73"/>
@@ -18589,11 +18651,11 @@
       </c>
       <c r="I47" s="72">
         <f>H47/($H$3)</f>
-        <v>-9.3481352667659223E-2</v>
+        <v>-9.337114349895459E-2</v>
       </c>
       <c r="J47" s="37" cm="1">
         <f t="array" ref="J47">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-9.3481352667659223E-2</v>
+        <v>-9.337114349895459E-2</v>
       </c>
       <c r="K47" t="str" cm="1">
         <f t="array" ref="K47">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -18605,7 +18667,7 @@
       </c>
       <c r="M47" s="73" cm="1">
         <f t="array" ref="M47">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-9.0952571433409266E-3</v>
+        <v>-9.1388734612279227E-3</v>
       </c>
       <c r="N47" s="73"/>
       <c r="O47" s="73"/>
@@ -18653,11 +18715,11 @@
       </c>
       <c r="I48" s="72">
         <f>H48/($H$3)</f>
-        <v>-0.12712843063636511</v>
+        <v>-0.12697855348697287</v>
       </c>
       <c r="J48" s="37" cm="1">
         <f t="array" ref="J48">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-0.12712843063636511</v>
+        <v>-0.12697855348697287</v>
       </c>
       <c r="K48" t="str" cm="1">
         <f t="array" ref="K48">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -18669,7 +18731,7 @@
       </c>
       <c r="M48" s="73" cm="1">
         <f t="array" ref="M48">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-1.2368945611835831E-2</v>
+        <v>-1.2428260907184876E-2</v>
       </c>
       <c r="N48" s="73"/>
       <c r="O48" s="73"/>
@@ -18717,11 +18779,11 @@
       </c>
       <c r="I49" s="72">
         <f>H49/($H$3)</f>
-        <v>-0.10427402129037688</v>
+        <v>-0.10415108818258631</v>
       </c>
       <c r="J49" s="37" cm="1">
         <f t="array" ref="J49">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-0.10427402129037688</v>
+        <v>-0.10415108818258631</v>
       </c>
       <c r="K49" t="str" cm="1">
         <f t="array" ref="K49">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -18733,7 +18795,7 @@
       </c>
       <c r="M49" s="73" cm="1">
         <f t="array" ref="M49">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-1.0145328559567282E-2</v>
+        <v>-1.0193980496345791E-2</v>
       </c>
       <c r="N49" s="73"/>
       <c r="O49" s="73"/>
@@ -18781,11 +18843,11 @@
       </c>
       <c r="I50" s="72">
         <f>H50/($H$3)</f>
-        <v>-1.8093284511332273E-2</v>
+        <v>-1.8071953563627449E-2</v>
       </c>
       <c r="J50" s="37" cm="1">
         <f t="array" ref="J50">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-1.8093284511332273E-2</v>
+        <v>-1.8071953563627449E-2</v>
       </c>
       <c r="K50" t="str" cm="1">
         <f t="array" ref="K50">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -18797,7 +18859,7 @@
       </c>
       <c r="M50" s="73" cm="1">
         <f t="array" ref="M50">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-1.7603839750077429E-3</v>
+        <v>-1.7688258987320577E-3</v>
       </c>
       <c r="N50" s="73"/>
       <c r="O50" s="73"/>
@@ -18845,11 +18907,11 @@
       </c>
       <c r="I51" s="72">
         <f>H51/($H$3)</f>
-        <v>-5.9675682775535852E-2</v>
+        <v>-5.9605328558326835E-2</v>
       </c>
       <c r="J51" s="37" cm="1">
         <f t="array" ref="J51">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-5.9675682775535852E-2</v>
+        <v>-5.9605328558326835E-2</v>
       </c>
       <c r="K51" t="str" cm="1">
         <f t="array" ref="K51">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -18861,7 +18923,7 @@
       </c>
       <c r="M51" s="73" cm="1">
         <f t="array" ref="M51">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-5.8061384924280686E-3</v>
+        <v>-5.833981837392436E-3</v>
       </c>
       <c r="N51" s="73"/>
       <c r="O51" s="73"/>
@@ -18909,11 +18971,11 @@
       </c>
       <c r="I52" s="72">
         <f>H52/($H$3)</f>
-        <v>-6.6976635377363675E-2</v>
+        <v>-6.6897673754570147E-2</v>
       </c>
       <c r="J52" s="37" cm="1">
         <f t="array" ref="J52">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-6.6976635377363675E-2</v>
+        <v>-6.6897673754570147E-2</v>
       </c>
       <c r="K52" t="str" cm="1">
         <f t="array" ref="K52">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -18925,7 +18987,7 @@
       </c>
       <c r="M52" s="73" cm="1">
         <f t="array" ref="M52">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-6.5164838116816828E-3</v>
+        <v>-6.5477336185817397E-3</v>
       </c>
       <c r="N52" s="73"/>
       <c r="O52" s="73"/>
@@ -18973,11 +19035,11 @@
       </c>
       <c r="I53" s="72">
         <f>H53/($H$3)</f>
-        <v>-8.4593470692017142E-2</v>
+        <v>-8.4493739827874087E-2</v>
       </c>
       <c r="J53" s="37" cm="1">
         <f t="array" ref="J53">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-8.4593470692017142E-2</v>
+        <v>-8.4493739827874087E-2</v>
       </c>
       <c r="K53" t="str" cm="1">
         <f t="array" ref="K53">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -18989,7 +19051,7 @@
       </c>
       <c r="M53" s="73" cm="1">
         <f t="array" ref="M53">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-8.2305117184911184E-3</v>
+        <v>-8.269981148527979E-3</v>
       </c>
       <c r="N53" s="73"/>
       <c r="O53" s="73"/>
@@ -19037,11 +19099,11 @@
       </c>
       <c r="I54" s="72">
         <f>H54/($H$3)</f>
-        <v>-8.8402707272955128E-2</v>
+        <v>-8.8298485536728991E-2</v>
       </c>
       <c r="J54" s="37" cm="1">
         <f t="array" ref="J54">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-8.8402707272955128E-2</v>
+        <v>-8.8298485536728991E-2</v>
       </c>
       <c r="K54" t="str" cm="1">
         <f t="array" ref="K54">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -19053,7 +19115,7 @@
       </c>
       <c r="M54" s="73" cm="1">
         <f t="array" ref="M54">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-8.6011309407719901E-3</v>
+        <v>-8.6423776757887181E-3</v>
       </c>
       <c r="N54" s="73"/>
       <c r="O54" s="73"/>
@@ -19101,11 +19163,11 @@
       </c>
       <c r="I55" s="72">
         <f>H55/($H$3)</f>
-        <v>-1.0316219426038862E-2</v>
+        <v>-1.0304057193308229E-2</v>
       </c>
       <c r="J55" s="37" cm="1">
         <f t="array" ref="J55">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-1.0316219426038862E-2</v>
+        <v>-1.0304057193308229E-2</v>
       </c>
       <c r="K55" t="str" cm="1">
         <f t="array" ref="K55">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -19117,7 +19179,7 @@
       </c>
       <c r="M55" s="73" cm="1">
         <f t="array" ref="M55">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-1.0037153480280494E-3</v>
+        <v>-1.0085286663320512E-3</v>
       </c>
       <c r="N55" s="73"/>
       <c r="O55" s="73"/>
@@ -19165,11 +19227,11 @@
       </c>
       <c r="I56" s="72">
         <f>H56/($H$3)</f>
-        <v>-3.110758691474725E-2</v>
+        <v>-3.1070912848781714E-2</v>
       </c>
       <c r="J56" s="37" cm="1">
         <f t="array" ref="J56">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-3.110758691474725E-2</v>
+        <v>-3.1070912848781714E-2</v>
       </c>
       <c r="K56" t="str" cm="1">
         <f t="array" ref="K56">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -19181,7 +19243,7 @@
       </c>
       <c r="M56" s="73" cm="1">
         <f t="array" ref="M56">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-3.0266089869743248E-3</v>
+        <v>-3.0411230944497976E-3</v>
       </c>
       <c r="N56" s="73"/>
       <c r="O56" s="73"/>
@@ -19229,11 +19291,11 @@
       </c>
       <c r="I57" s="72">
         <f>H57/($H$3)</f>
-        <v>-0.11633609872686067</v>
+        <v>-0.11619894511958875</v>
       </c>
       <c r="J57" s="37" cm="1">
         <f t="array" ref="J57">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-0.11633609872686067</v>
+        <v>-0.11619894511958875</v>
       </c>
       <c r="K57" t="str" cm="1">
         <f t="array" ref="K57">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -19245,7 +19307,7 @@
       </c>
       <c r="M57" s="73" cm="1">
         <f t="array" ref="M57">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-1.1318906956081702E-2</v>
+        <v>-1.1373186789642125E-2</v>
       </c>
       <c r="N57" s="73"/>
       <c r="O57" s="73"/>
@@ -19293,11 +19355,11 @@
       </c>
       <c r="I58" s="72">
         <f>H58/($H$3)</f>
-        <v>-3.1564170031847215E-2</v>
+        <v>-3.1526957680498083E-2</v>
       </c>
       <c r="J58" s="37" cm="1">
         <f t="array" ref="J58">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-3.1564170031847215E-2</v>
+        <v>-3.1526957680498083E-2</v>
       </c>
       <c r="K58" t="str" cm="1">
         <f t="array" ref="K58">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -19309,13 +19371,22 @@
       </c>
       <c r="M58" s="73" cm="1">
         <f t="array" ref="M58">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-3.1564170031847215E-2</v>
+        <v>-3.1526957680498083E-2</v>
       </c>
       <c r="N58" s="73"/>
       <c r="O58" s="73"/>
-      <c r="P58" s="73"/>
-      <c r="Q58" s="73"/>
-      <c r="R58" s="73"/>
+      <c r="P58" s="73" t="str" cm="1">
+        <f t="array" ref="P58:P61">B58:B61</f>
+        <v>ctp_c</v>
+      </c>
+      <c r="Q58" s="103" cm="1">
+        <f t="array" ref="Q58:Q60">F58:F60</f>
+        <v>-9.3742000000000006E-2</v>
+      </c>
+      <c r="R58" s="73" cm="1">
+        <f t="array" ref="R58:R61">Q58:Q61*E58:E61/1000</f>
+        <v>-2.8513813582342007E-2</v>
+      </c>
       <c r="S58" s="73"/>
       <c r="T58" s="73"/>
       <c r="U58" s="73"/>
@@ -19355,11 +19426,11 @@
       </c>
       <c r="I59" s="72">
         <f>H59/($H$3)</f>
-        <v>-3.2482386964245151E-2</v>
+        <v>-3.2444092087644483E-2</v>
       </c>
       <c r="J59" s="37" cm="1">
         <f t="array" ref="J59">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-3.2482386964245151E-2</v>
+        <v>-3.2444092087644483E-2</v>
       </c>
       <c r="K59" t="str" cm="1">
         <f t="array" ref="K59">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -19371,13 +19442,19 @@
       </c>
       <c r="M59" s="73" cm="1">
         <f t="array" ref="M59">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-3.2482386964245151E-2</v>
+        <v>-3.2444092087644483E-2</v>
       </c>
       <c r="N59" s="73"/>
       <c r="O59" s="73"/>
-      <c r="P59" s="73"/>
-      <c r="Q59" s="73"/>
-      <c r="R59" s="73"/>
+      <c r="P59" s="73" t="str">
+        <v>gtp_c</v>
+      </c>
+      <c r="Q59" s="73">
+        <v>-9.6468999999999999E-2</v>
+      </c>
+      <c r="R59" s="73">
+        <v>-3.3204379077068996E-2</v>
+      </c>
       <c r="S59" s="73"/>
       <c r="T59" s="73"/>
       <c r="U59" s="73"/>
@@ -19417,11 +19494,11 @@
       </c>
       <c r="I60" s="72">
         <f>H60/($H$3)</f>
-        <v>-4.2297577129041579E-2</v>
+        <v>-4.2247710704555998E-2</v>
       </c>
       <c r="J60" s="37" cm="1">
         <f t="array" ref="J60">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-4.2297577129041579E-2</v>
+        <v>-4.2247710704555998E-2</v>
       </c>
       <c r="K60" t="str" cm="1">
         <f t="array" ref="K60">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -19433,13 +19510,19 @@
       </c>
       <c r="M60" s="73" cm="1">
         <f t="array" ref="M60">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-4.2297577129041579E-2</v>
+        <v>-4.2247710704555998E-2</v>
       </c>
       <c r="N60" s="73"/>
       <c r="O60" s="73"/>
-      <c r="P60" s="73"/>
-      <c r="Q60" s="73"/>
-      <c r="R60" s="73"/>
+      <c r="P60" s="73" t="str">
+        <v>utp_c</v>
+      </c>
+      <c r="Q60" s="73">
+        <v>-0.12561900000000001</v>
+      </c>
+      <c r="R60" s="73">
+        <v>-3.8333650464758999E-2</v>
+      </c>
       <c r="S60" s="73"/>
       <c r="T60" s="73"/>
       <c r="U60" s="73"/>
@@ -19479,11 +19562,11 @@
       </c>
       <c r="I61" s="72">
         <f>H61/($H$3)</f>
-        <v>-1.6161123080023454</v>
+        <v>-1.6142070040148062</v>
       </c>
       <c r="J61" s="37" cm="1">
         <f t="array" ref="J61">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-130.33905430800235</v>
+        <v>-130.3371490040148</v>
       </c>
       <c r="K61" t="str" cm="1">
         <f t="array" ref="K61">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -19495,13 +19578,20 @@
       </c>
       <c r="M61" s="73" cm="1">
         <f t="array" ref="M61">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-141.07905430800236</v>
+        <v>-141.07714900401481</v>
       </c>
       <c r="N61" s="73"/>
       <c r="O61" s="73"/>
-      <c r="P61" s="73"/>
-      <c r="Q61" s="73"/>
-      <c r="R61" s="73"/>
+      <c r="P61" s="73" t="str">
+        <v>atp_c</v>
+      </c>
+      <c r="Q61" s="73">
+        <f>Q60</f>
+        <v>-0.12561900000000001</v>
+      </c>
+      <c r="R61" s="73">
+        <v>-4.1227904687618999E-2</v>
+      </c>
       <c r="S61" s="73"/>
       <c r="T61" s="73"/>
       <c r="U61" s="73"/>
@@ -19541,11 +19631,11 @@
       </c>
       <c r="I62" s="72">
         <f>H62/($H$3)</f>
-        <v>-1.0513196655761193E-2</v>
+        <v>-1.0500802198141618E-2</v>
       </c>
       <c r="J62" s="37" cm="1">
         <f t="array" ref="J62">_xlfn.LET(_xlpm.id,mets27138[[#This Row],[name w/o location]],_xlpm.oldcoeff,mets27138[[#This Row],[normalized coeffs]],_xlpm.gam,$J$2-$G$2,_xlfn.IFS(IFERROR(MATCH(_xlpm.id,{"atp","h2o"},0),0)&gt;0,_xlpm.oldcoeff-_xlpm.gam,IFERROR(MATCH(_xlpm.id,{"adp","h","pi"},0),0)&gt;0,_xlpm.oldcoeff+_xlpm.gam,TRUE,_xlpm.oldcoeff))</f>
-        <v>-1.0513196655761193E-2</v>
+        <v>-1.0500802198141618E-2</v>
       </c>
       <c r="K62" t="str" cm="1">
         <f t="array" ref="K62">"BIOSYN-"&amp;_xlfn.IFS(IFERROR(MATCH(mets27138[[#This Row],[category]],{0,"0",""},0),0)&gt;0,mets27138[[#This Row],[name]],TRUE,mets27138[[#This Row],[category]]&amp;"-"&amp;mets27138[[#This Row],[name]])</f>
@@ -19557,7 +19647,7 @@
       </c>
       <c r="M62" s="73" cm="1">
         <f t="array" ref="M62">_xlfn.LET(_xlpm.gam,$J$2,_xlpm.cat,IF(LEFT(mets27138[[#This Row],[name w/o location]],4)="trna","PROT",mets27138[[#This Row],[category]]),_xlpm.multipliers,_xlfn._xlws.FILTER(_xlfn.HSTACK(biomassComponents26127[normalized coeffs],biomassComponents26127[original coeffs from input]),(biomassComponents26127[rxn name]="BIOSYN-"&amp;_xlpm.cat)+IF(mets27138[[#This Row],[name w/o location]]="ppi",((biomassComponents26127[rxn name]="BIOSYN-DNA"))+((biomassComponents26127[rxn name]="BIOSYN-RNA"))&gt;0,FALSE),{1,1}),mets27138[[#This Row],[normalized coeffs]]*(SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,1))/SUM(_xlfn.CHOOSECOLS(_xlpm.multipliers,2)))+_xlfn.IFS(OR(mets27138[[#This Row],[name w/o location]]={"atp","h2o"}),-_xlpm.gam,OR(mets27138[[#This Row],[name w/o location]]={"adp","h","pi"}),_xlpm.gam,TRUE,0))</f>
-        <v>-1.0513196655761193E-2</v>
+        <v>-1.0500802198141618E-2</v>
       </c>
       <c r="N62" s="73"/>
       <c r="O62" s="73"/>
@@ -19604,7 +19694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042FF932-C48A-D446-979E-E5F082761A47}">
   <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A84" workbookViewId="0">
       <selection activeCell="A71" sqref="A54:D71"/>
     </sheetView>
   </sheetViews>
@@ -21423,8 +21513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5455B0F7-CD7B-1440-98EA-12626AC5D91D}">
   <dimension ref="A1:K135"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G116" sqref="G116:G135"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>